<commit_message>
added model for all data at once
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{711F0276-BBCB-064E-99BA-32E791ACD4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD36A117-CC09-A84E-9710-A929416FA8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="920" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
+    <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="82">
   <si>
     <t>Model</t>
   </si>
@@ -59,9 +59,6 @@
     <t>0.621 (0.019)</t>
   </si>
   <si>
-    <t>Log Reg</t>
-  </si>
-  <si>
     <t>PCA</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>Val AUC C_2</t>
+  </si>
+  <si>
+    <t>2023-03-03-2123_Log_Reg_all.csv</t>
   </si>
 </sst>
 </file>
@@ -343,8 +343,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N20" totalsRowShown="0">
-  <autoFilter ref="A1:N20" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N21" totalsRowShown="0">
+  <autoFilter ref="A1:N21" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -662,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,43 +686,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
         <v>79</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>80</v>
-      </c>
-      <c r="K1" t="s">
-        <v>81</v>
       </c>
       <c r="L1" t="s">
         <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N1" t="s">
         <v>3</v>
@@ -730,31 +730,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
       <c r="M2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N2">
         <v>0.6018</v>
@@ -762,31 +762,31 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>53</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" t="s">
-        <v>54</v>
       </c>
       <c r="N3">
         <v>0.64300000000000002</v>
@@ -794,31 +794,31 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N4">
         <v>0.61199999999999999</v>
@@ -826,31 +826,31 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N5">
         <v>0.58799999999999997</v>
@@ -858,31 +858,31 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="L6" t="s">
-        <v>44</v>
-      </c>
       <c r="M6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N6">
         <v>0.53900000000000003</v>
@@ -890,31 +890,31 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N7">
         <v>0.57199999999999995</v>
@@ -922,60 +922,60 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N9">
         <v>0.63100000000000001</v>
@@ -983,31 +983,31 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N10">
         <v>0.58699999999999997</v>
@@ -1015,31 +1015,31 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N11">
         <v>0.59899999999999998</v>
@@ -1047,31 +1047,31 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N12">
         <v>0.60099999999999998</v>
@@ -1079,31 +1079,31 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N13">
         <v>0.60499999999999998</v>
@@ -1111,31 +1111,31 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N14">
         <v>0.59099999999999997</v>
@@ -1143,25 +1143,25 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I15">
         <v>0.63200000000000001</v>
@@ -1176,7 +1176,7 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N15">
         <v>0.59799999999999998</v>
@@ -1184,25 +1184,25 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I16">
         <v>0.628</v>
@@ -1217,7 +1217,7 @@
         <v>4</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N16">
         <v>0.59399999999999997</v>
@@ -1225,22 +1225,22 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G17">
         <v>50</v>
@@ -1258,7 +1258,7 @@
         <v>6</v>
       </c>
       <c r="M17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N17">
         <v>0.55800000000000005</v>
@@ -1266,22 +1266,22 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18">
         <v>0.59699999999999998</v>
@@ -1290,7 +1290,7 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="M18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N18">
         <v>0.51600000000000001</v>
@@ -1298,22 +1298,22 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19">
         <v>0.64700000000000002</v>
@@ -1324,28 +1324,48 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20">
         <v>0.61899999999999999</v>
       </c>
       <c r="K20">
         <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added LogReg and RF submission with all data
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD36A117-CC09-A84E-9710-A929416FA8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379383B5-A0EB-5147-8ADD-EE2FB653957F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
   <si>
     <t>Model</t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>2023-03-03-2123_Log_Reg_all.csv</t>
+  </si>
+  <si>
+    <t>2023-03-04-2149_RF_all.csv</t>
+  </si>
+  <si>
+    <t>March 4, 2023, 8:50 p.m.</t>
+  </si>
+  <si>
+    <t>March 4, 2023, 8:35 p.m.</t>
   </si>
 </sst>
 </file>
@@ -343,8 +352,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N21" totalsRowShown="0">
-  <autoFilter ref="A1:N21" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N22" totalsRowShown="0">
+  <autoFilter ref="A1:N22" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -662,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
         <v>52</v>
@@ -1307,7 +1316,7 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
         <v>52</v>
@@ -1333,7 +1342,7 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>52</v>
@@ -1359,13 +1368,45 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
         <v>52</v>
       </c>
       <c r="F21" t="s">
         <v>40</v>
+      </c>
+      <c r="M21" t="s">
+        <v>84</v>
+      </c>
+      <c r="N21">
+        <v>0.64700000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" t="s">
+        <v>83</v>
+      </c>
+      <c r="N22">
+        <v>0.60299999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated submission tracker with center only submissions and tuned log reg
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379383B5-A0EB-5147-8ADD-EE2FB653957F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE52CEC-48C0-594C-B640-E2B6B230152E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
   <si>
     <t>Model</t>
   </si>
@@ -291,6 +291,27 @@
   </si>
   <si>
     <t>March 4, 2023, 8:35 p.m.</t>
+  </si>
+  <si>
+    <t>March 5, 2023, 8:36 p.m.</t>
+  </si>
+  <si>
+    <t>March 5, 2023, 8:51 p.m.</t>
+  </si>
+  <si>
+    <t>March 7, 2023, 9:56 p.m.</t>
+  </si>
+  <si>
+    <t>{'C': 0.6, 'max_iter': 100, 'penalty': 'l2', 'solver': 'lbfgs'}</t>
+  </si>
+  <si>
+    <t>2023-03-07-2255_tuned_LogReg.csv</t>
+  </si>
+  <si>
+    <t>March 7, 2023, 5:46 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-07-1846_LogReg_C5.csv</t>
   </si>
 </sst>
 </file>
@@ -352,8 +373,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N22" totalsRowShown="0">
-  <autoFilter ref="A1:N22" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N24" totalsRowShown="0">
+  <autoFilter ref="A1:N24" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -671,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1330,6 +1351,12 @@
       <c r="K19">
         <v>0.58699999999999997</v>
       </c>
+      <c r="M19" t="s">
+        <v>85</v>
+      </c>
+      <c r="N19">
+        <v>0.51800000000000002</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1356,6 +1383,12 @@
       <c r="K20">
         <v>0.58199999999999996</v>
       </c>
+      <c r="M20" t="s">
+        <v>86</v>
+      </c>
+      <c r="N20">
+        <v>0.66600000000000004</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1407,6 +1440,61 @@
       </c>
       <c r="N22">
         <v>0.60299999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>88</v>
+      </c>
+      <c r="M23" t="s">
+        <v>87</v>
+      </c>
+      <c r="N23">
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" t="s">
+        <v>90</v>
+      </c>
+      <c r="N24">
+        <v>0.624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to model on only C1 & C 5 for LogReg and RF
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE52CEC-48C0-594C-B640-E2B6B230152E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D5D045-6002-9C44-954A-D30D81F64182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="96">
   <si>
     <t>Model</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>2023-03-07-1846_LogReg_C5.csv</t>
+  </si>
+  <si>
+    <t>2023-03-09-1316_RF_C1_C5.csv</t>
+  </si>
+  <si>
+    <t>2023-03-09-1310_LogReg_C1_C5.csv</t>
+  </si>
+  <si>
+    <t>March 9, 2023, 12:11 p.m.</t>
+  </si>
+  <si>
+    <t>March 9, 2023, 12:16 p.m.</t>
   </si>
 </sst>
 </file>
@@ -373,8 +385,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N24" totalsRowShown="0">
-  <autoFilter ref="A1:N24" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N26" totalsRowShown="0">
+  <autoFilter ref="A1:N26" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -692,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1497,6 +1509,64 @@
         <v>0.624</v>
       </c>
     </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="M25" t="s">
+        <v>94</v>
+      </c>
+      <c r="N25">
+        <v>0.63100000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="M26" t="s">
+        <v>95</v>
+      </c>
+      <c r="N26">
+        <v>0.60299999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added test runs for averaged moco features
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D5D045-6002-9C44-954A-D30D81F64182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522EA697-B578-C942-97A6-79EA6F363758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="110">
   <si>
     <t>Model</t>
   </si>
@@ -324,6 +324,48 @@
   </si>
   <si>
     <t>March 9, 2023, 12:16 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-09-1515_RF_scaled_center.csv</t>
+  </si>
+  <si>
+    <t>2023-03-09-1501_LogReg_scaled_center.csv</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>scaled every center data separately and submission on all</t>
+  </si>
+  <si>
+    <t>March 9, 2023, 2:13 p.m.</t>
+  </si>
+  <si>
+    <t>March 9, 2023, 2:17 p.m.</t>
+  </si>
+  <si>
+    <t>submission on C1 &amp; C5 only</t>
+  </si>
+  <si>
+    <t>submission on C2 only</t>
+  </si>
+  <si>
+    <t>submission on C1 only</t>
+  </si>
+  <si>
+    <t>submission on C5 only</t>
+  </si>
+  <si>
+    <t>0.645 (0.039)</t>
+  </si>
+  <si>
+    <t>0.630 (0.046)</t>
+  </si>
+  <si>
+    <t>{"max_depth": 3}</t>
+  </si>
+  <si>
+    <t>0.659 (0.039)</t>
   </si>
 </sst>
 </file>
@@ -385,9 +427,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:N26" totalsRowShown="0">
-  <autoFilter ref="A1:N26" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O31" totalsRowShown="0">
+  <autoFilter ref="A1:O31" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
     <tableColumn id="3" xr3:uid="{A38F4111-BA96-B34B-ABA6-3C86C9C9AFB0}" name="Data"/>
@@ -396,6 +438,7 @@
     <tableColumn id="6" xr3:uid="{3AD5D56C-379A-CD4B-BBBF-A5CCFA8A0931}" name="Grade weakly supervision"/>
     <tableColumn id="7" xr3:uid="{A896B93D-0FBB-0B4B-906A-D3D50CFC09B8}" name="PCA"/>
     <tableColumn id="8" xr3:uid="{D8F24906-51F8-AB44-9001-6E82316E59D5}" name="Hyperparameters"/>
+    <tableColumn id="15" xr3:uid="{B9980961-6BAB-DC4D-B74E-BEC095DB7AA7}" name="Comments"/>
     <tableColumn id="9" xr3:uid="{C3652559-D067-784E-BB5A-A2350D8190DB}" name="Val AUC C_1"/>
     <tableColumn id="10" xr3:uid="{21A7BD43-54F6-C341-9F74-F1645DAD5250}" name="Val AUC C_5"/>
     <tableColumn id="11" xr3:uid="{74373329-BF49-8840-BB75-12B22AA73521}" name="Val AUC C_2"/>
@@ -704,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="B31" sqref="B31:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,13 +763,14 @@
     <col min="6" max="6" width="41.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" customWidth="1"/>
     <col min="8" max="8" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="9" max="9" width="46.33203125" customWidth="1"/>
+    <col min="10" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -752,25 +796,28 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>79</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>80</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -792,17 +839,17 @@
       <c r="H2" t="s">
         <v>52</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2">
+      <c r="N2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2">
         <v>0.6018</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -824,17 +871,17 @@
       <c r="H3" t="s">
         <v>52</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>53</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.64300000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -856,17 +903,17 @@
       <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>54</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.61199999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -888,17 +935,17 @@
       <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>17</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>55</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0.58799999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -920,17 +967,17 @@
       <c r="H6" t="s">
         <v>72</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>43</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>56</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -952,17 +999,17 @@
       <c r="H7" t="s">
         <v>73</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>44</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>57</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0.57199999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -984,14 +1031,14 @@
       <c r="H8" t="s">
         <v>74</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>45</v>
       </c>
-      <c r="M8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1013,17 +1060,26 @@
       <c r="H9" t="s">
         <v>52</v>
       </c>
-      <c r="L9" t="s">
+      <c r="J9">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="K9">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="L9">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="M9" t="s">
         <v>46</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>58</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>0.63100000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1045,17 +1101,17 @@
       <c r="H10" t="s">
         <v>74</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>47</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>59</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>0.58699999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1077,17 +1133,17 @@
       <c r="H11" t="s">
         <v>52</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>48</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>60</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>0.59899999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1109,17 +1165,26 @@
       <c r="H12" t="s">
         <v>52</v>
       </c>
-      <c r="L12" t="s">
+      <c r="J12">
+        <v>0.628</v>
+      </c>
+      <c r="K12">
+        <v>0.62</v>
+      </c>
+      <c r="L12">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="M12" t="s">
         <v>49</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>61</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0.60099999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1141,17 +1206,17 @@
       <c r="H13" t="s">
         <v>52</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>50</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>62</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1173,17 +1238,17 @@
       <c r="H14" t="s">
         <v>75</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>51</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>63</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1205,26 +1270,26 @@
       <c r="H15" t="s">
         <v>76</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.63200000000000001</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>0.63</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0.59899999999999998</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>1</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>64</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1246,26 +1311,26 @@
       <c r="H16" t="s">
         <v>77</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>0.628</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>0.63</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>0.60799999999999998</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>4</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>65</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>0.59399999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1287,26 +1352,26 @@
       <c r="G17">
         <v>50</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.626</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>0.64100000000000001</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>0.59599999999999997</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>6</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>66</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1325,20 +1390,23 @@
       <c r="F18" t="s">
         <v>40</v>
       </c>
-      <c r="I18">
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18">
         <v>0.59699999999999998</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>0.60799999999999998</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>67</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>0.51600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1357,20 +1425,23 @@
       <c r="F19" t="s">
         <v>40</v>
       </c>
-      <c r="J19">
+      <c r="I19" t="s">
+        <v>104</v>
+      </c>
+      <c r="K19">
         <v>0.64700000000000002</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>0.58699999999999997</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>85</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>0.51800000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1389,20 +1460,23 @@
       <c r="F20" t="s">
         <v>40</v>
       </c>
-      <c r="I20">
+      <c r="I20" t="s">
+        <v>105</v>
+      </c>
+      <c r="J20">
         <v>0.61899999999999999</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>0.58199999999999996</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>86</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -1421,14 +1495,14 @@
       <c r="F21" t="s">
         <v>40</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>84</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>0.64700000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1447,14 +1521,14 @@
       <c r="F22" t="s">
         <v>40</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>83</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>0.60299999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -1476,14 +1550,14 @@
       <c r="H23" t="s">
         <v>88</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>87</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>0.64600000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>91</v>
       </c>
@@ -1502,14 +1576,14 @@
       <c r="F24" t="s">
         <v>40</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>90</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>0.624</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>93</v>
       </c>
@@ -1528,17 +1602,20 @@
       <c r="F25" t="s">
         <v>40</v>
       </c>
-      <c r="K25">
+      <c r="I25" t="s">
+        <v>102</v>
+      </c>
+      <c r="L25">
         <v>0.60899999999999999</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>94</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>0.63100000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -1557,14 +1634,165 @@
       <c r="F26" t="s">
         <v>40</v>
       </c>
-      <c r="K26">
+      <c r="I26" t="s">
+        <v>102</v>
+      </c>
+      <c r="L26">
         <v>0.58599999999999997</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>95</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>0.60299999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27" t="s">
+        <v>99</v>
+      </c>
+      <c r="N27" t="s">
+        <v>100</v>
+      </c>
+      <c r="O27">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" t="s">
+        <v>99</v>
+      </c>
+      <c r="N28" t="s">
+        <v>101</v>
+      </c>
+      <c r="O28">
+        <v>0.61199999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="K29">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="L29">
+        <v>0.628</v>
+      </c>
+      <c r="M29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="K30">
+        <v>0.69</v>
+      </c>
+      <c r="L30">
+        <v>0.62</v>
+      </c>
+      <c r="M30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
+        <v>39</v>
+      </c>
+      <c r="H31" t="s">
+        <v>108</v>
+      </c>
+      <c r="J31">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="K31">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="L31">
+        <v>0.68</v>
+      </c>
+      <c r="M31" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
full data tile avg submissions
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522EA697-B578-C942-97A6-79EA6F363758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46761D7-8DAF-8744-A821-AFC60EE816FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="114">
   <si>
     <t>Model</t>
   </si>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t>0.659 (0.039)</t>
+  </si>
+  <si>
+    <t>submission trained on all data</t>
+  </si>
+  <si>
+    <t>2023-03-09-1757_LogReg_tile_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-09-1800_RF_tile_avg.csv</t>
+  </si>
+  <si>
+    <t>March 9</t>
   </si>
 </sst>
 </file>
@@ -749,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:F31"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1706,6 +1718,9 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>111</v>
+      </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
@@ -1721,6 +1736,9 @@
       <c r="F29" t="s">
         <v>39</v>
       </c>
+      <c r="I29" t="s">
+        <v>110</v>
+      </c>
       <c r="J29">
         <v>0.60899999999999999</v>
       </c>
@@ -1733,8 +1751,17 @@
       <c r="M29" t="s">
         <v>106</v>
       </c>
+      <c r="N29" t="s">
+        <v>113</v>
+      </c>
+      <c r="O29">
+        <v>0.58699999999999997</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>112</v>
+      </c>
       <c r="B30" t="s">
         <v>38</v>
       </c>
@@ -1750,6 +1777,9 @@
       <c r="F30" t="s">
         <v>39</v>
       </c>
+      <c r="I30" t="s">
+        <v>110</v>
+      </c>
       <c r="J30">
         <v>0.57899999999999996</v>
       </c>
@@ -1761,6 +1791,12 @@
       </c>
       <c r="M30" t="s">
         <v>107</v>
+      </c>
+      <c r="N30" t="s">
+        <v>113</v>
+      </c>
+      <c r="O30">
+        <v>0.63300000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
more model test runs on the avg moco tile features for tree models
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46761D7-8DAF-8744-A821-AFC60EE816FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB788440-4537-4242-8045-EBDB7F3307C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="123">
   <si>
     <t>Model</t>
   </si>
@@ -378,6 +378,33 @@
   </si>
   <si>
     <t>March 9</t>
+  </si>
+  <si>
+    <t>0.649 (0.040)</t>
+  </si>
+  <si>
+    <t>0.644 (0.045)</t>
+  </si>
+  <si>
+    <t>Catboost</t>
+  </si>
+  <si>
+    <t>0.654 (0.043)</t>
+  </si>
+  <si>
+    <t>LightGBM</t>
+  </si>
+  <si>
+    <t>ExtraTrees</t>
+  </si>
+  <si>
+    <t>0.624 (0.021)</t>
+  </si>
+  <si>
+    <t>DecisionTree</t>
+  </si>
+  <si>
+    <t>0.532 (0.024)</t>
   </si>
 </sst>
 </file>
@@ -439,8 +466,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O31" totalsRowShown="0">
-  <autoFilter ref="A1:O31" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O36" totalsRowShown="0">
+  <autoFilter ref="A1:O36" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -759,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1831,6 +1858,151 @@
         <v>109</v>
       </c>
     </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K32">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="L32">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="M32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33">
+        <v>0.63</v>
+      </c>
+      <c r="K33">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="L33">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="M33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="K34">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="L34">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="M34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="K35">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="L35">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="M35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36">
+        <v>0.505</v>
+      </c>
+      <c r="K36">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="L36">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="M36" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added submissions for restricted RF on averaged data
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB788440-4537-4242-8045-EBDB7F3307C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A38DF4B-8F83-4140-861C-00013C3CFCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="128">
   <si>
     <t>Model</t>
   </si>
@@ -405,13 +405,28 @@
   </si>
   <si>
     <t>0.532 (0.024)</t>
+  </si>
+  <si>
+    <t>2023-03-10-1326_RF_avg_restricted.csv</t>
+  </si>
+  <si>
+    <t>March 10, 2023, 12:27 p.m.</t>
+  </si>
+  <si>
+    <t>0.639 (0.068)</t>
+  </si>
+  <si>
+    <t>March 10, 2023, 12:34 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-10-1333_RF_avg_restricted_cv.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -425,6 +440,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -434,7 +456,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -442,12 +464,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -466,8 +500,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O36" totalsRowShown="0">
-  <autoFilter ref="A1:O36" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O38" totalsRowShown="0">
+  <autoFilter ref="A1:O38" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -786,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1887,7 +1921,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>116</v>
       </c>
@@ -1916,7 +1950,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>118</v>
       </c>
@@ -1945,7 +1979,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>119</v>
       </c>
@@ -1974,7 +2008,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>121</v>
       </c>
@@ -2001,6 +2035,79 @@
       </c>
       <c r="M36" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" t="s">
+        <v>39</v>
+      </c>
+      <c r="H37" t="s">
+        <v>108</v>
+      </c>
+      <c r="I37" t="s">
+        <v>110</v>
+      </c>
+      <c r="N37" t="s">
+        <v>124</v>
+      </c>
+      <c r="O37">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J38">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="K38">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="L38">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="M38" t="s">
+        <v>125</v>
+      </c>
+      <c r="N38" t="s">
+        <v>126</v>
+      </c>
+      <c r="O38">
+        <v>0.60299999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scaling test run for weakly logReg and RF as well as played with cv for RF averaged
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A38DF4B-8F83-4140-861C-00013C3CFCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2844D328-4F84-8E45-8502-F0805B73D9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="131">
   <si>
     <t>Model</t>
   </si>
@@ -420,6 +420,15 @@
   </si>
   <si>
     <t>2023-03-10-1333_RF_avg_restricted_cv.csv</t>
+  </si>
+  <si>
+    <t>0.653 (0.054)</t>
+  </si>
+  <si>
+    <t>0.645 (0.043)</t>
+  </si>
+  <si>
+    <t>0.600 (0.024)</t>
   </si>
 </sst>
 </file>
@@ -500,8 +509,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O38" totalsRowShown="0">
-  <autoFilter ref="A1:O38" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O39" totalsRowShown="0">
+  <autoFilter ref="A1:O39" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -820,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1742,6 +1751,18 @@
       <c r="I27" t="s">
         <v>99</v>
       </c>
+      <c r="J27">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="K27">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="L27">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="M27" t="s">
+        <v>130</v>
+      </c>
       <c r="N27" t="s">
         <v>100</v>
       </c>
@@ -1771,6 +1792,18 @@
       <c r="I28" t="s">
         <v>99</v>
       </c>
+      <c r="J28">
+        <v>0.629</v>
+      </c>
+      <c r="K28">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="L28">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="M28" t="s">
+        <v>129</v>
+      </c>
       <c r="N28" t="s">
         <v>101</v>
       </c>
@@ -2108,6 +2141,35 @@
       </c>
       <c r="O38">
         <v>0.60299999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39">
+        <v>0.6</v>
+      </c>
+      <c r="K39">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="L39">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="M39" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
performed test runs for averged LogReg & RF with center scaled data
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2844D328-4F84-8E45-8502-F0805B73D9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6B0426-9D3C-3E4D-9C3C-A34F149A7816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="134">
   <si>
     <t>Model</t>
   </si>
@@ -429,6 +429,15 @@
   </si>
   <si>
     <t>0.600 (0.024)</t>
+  </si>
+  <si>
+    <t>0.647 (0.030)</t>
+  </si>
+  <si>
+    <t>scaled every center data before average</t>
+  </si>
+  <si>
+    <t>0.648 (0.024)</t>
   </si>
 </sst>
 </file>
@@ -509,8 +518,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O39" totalsRowShown="0">
-  <autoFilter ref="A1:O39" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O41" totalsRowShown="0">
+  <autoFilter ref="A1:O41" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -829,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2172,6 +2181,70 @@
         <v>128</v>
       </c>
     </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
+        <v>39</v>
+      </c>
+      <c r="I40" t="s">
+        <v>132</v>
+      </c>
+      <c r="J40">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="K40">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="L40">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="M40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" t="s">
+        <v>132</v>
+      </c>
+      <c r="J41">
+        <v>0.64</v>
+      </c>
+      <c r="K41">
+        <v>0.68</v>
+      </c>
+      <c r="L41">
+        <v>0.624</v>
+      </c>
+      <c r="M41" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added results of scaled avg RF & LogReg
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6B0426-9D3C-3E4D-9C3C-A34F149A7816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D739D26-2049-3D4F-ADC1-C97F1DB5ED48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="136">
   <si>
     <t>Model</t>
   </si>
@@ -434,10 +434,16 @@
     <t>0.647 (0.030)</t>
   </si>
   <si>
-    <t>scaled every center data before average</t>
-  </si>
-  <si>
     <t>0.648 (0.024)</t>
+  </si>
+  <si>
+    <t>scaled every center data before average; submission trained on all data</t>
+  </si>
+  <si>
+    <t>March 10, 2023, 4:30 p.m.</t>
+  </si>
+  <si>
+    <t>March 10, 2023, 4:31 p.m.</t>
   </si>
 </sst>
 </file>
@@ -504,7 +510,418 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -840,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" topLeftCell="H9" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2198,7 +2615,7 @@
         <v>39</v>
       </c>
       <c r="I40" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J40">
         <v>0.61599999999999999</v>
@@ -2211,6 +2628,12 @@
       </c>
       <c r="M40" t="s">
         <v>131</v>
+      </c>
+      <c r="N40" t="s">
+        <v>135</v>
+      </c>
+      <c r="O40">
+        <v>0.64900000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2230,7 +2653,7 @@
         <v>39</v>
       </c>
       <c r="I41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J41">
         <v>0.64</v>
@@ -2242,11 +2665,37 @@
         <v>0.624</v>
       </c>
       <c r="M41" t="s">
-        <v>133</v>
+        <v>132</v>
+      </c>
+      <c r="N41" t="s">
+        <v>134</v>
+      </c>
+      <c r="O41">
+        <v>0.623</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="top10" dxfId="15" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="9" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="top10" dxfId="13" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="8" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="top10" dxfId="10" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K41">
+    <cfRule type="top10" dxfId="9" priority="7" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J41">
+    <cfRule type="top10" dxfId="8" priority="6" rank="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
test run for min max scaler before avg
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D739D26-2049-3D4F-ADC1-C97F1DB5ED48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2EFE28-ABF9-BF4C-A9BC-86DCF3698AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="139">
   <si>
     <t>Model</t>
   </si>
@@ -444,6 +444,15 @@
   </si>
   <si>
     <t>March 10, 2023, 4:31 p.m.</t>
+  </si>
+  <si>
+    <t>min max scaling center data before avg</t>
+  </si>
+  <si>
+    <t>0.635 (0.042)</t>
+  </si>
+  <si>
+    <t>0.669 (0.029)</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -528,66 +537,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -671,256 +620,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -935,8 +634,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O41" totalsRowShown="0">
-  <autoFilter ref="A1:O41" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O43" totalsRowShown="0">
+  <autoFilter ref="A1:O43" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1255,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H9" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2674,27 +2373,91 @@
         <v>0.623</v>
       </c>
     </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" t="s">
+        <v>39</v>
+      </c>
+      <c r="I42" t="s">
+        <v>136</v>
+      </c>
+      <c r="J42">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="K42">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="L42">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="M42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>39</v>
+      </c>
+      <c r="I43" t="s">
+        <v>136</v>
+      </c>
+      <c r="J43">
+        <v>0.64</v>
+      </c>
+      <c r="K43">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="L43">
+        <v>0.66</v>
+      </c>
+      <c r="M43" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="15" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="14" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="9" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="13" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="12" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="7" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="10" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K41">
-    <cfRule type="top10" dxfId="9" priority="7" rank="2"/>
+  <conditionalFormatting sqref="K2:K43">
+    <cfRule type="top10" dxfId="3" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J41">
-    <cfRule type="top10" dxfId="8" priority="6" rank="2"/>
+  <conditionalFormatting sqref="J2:J43">
+    <cfRule type="top10" dxfId="2" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
implemented choice of scaling - minmax vs standard
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2EFE28-ABF9-BF4C-A9BC-86DCF3698AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39EBC47-576E-A84E-A3EE-1D4A04D45B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="146">
   <si>
     <t>Model</t>
   </si>
@@ -453,6 +453,27 @@
   </si>
   <si>
     <t>0.669 (0.029)</t>
+  </si>
+  <si>
+    <t>0.654 (0.064)</t>
+  </si>
+  <si>
+    <t>standard scaling center data before avg</t>
+  </si>
+  <si>
+    <t>0.628 (0.015)</t>
+  </si>
+  <si>
+    <t>2023-03-10-1724_LogReg_scaled_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-10-1727_RF_scaled_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-10-1836_RF_minmax_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-10-1838_LogReg_minmax_avg.csv</t>
   </si>
 </sst>
 </file>
@@ -519,7 +540,67 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -634,8 +715,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O43" totalsRowShown="0">
-  <autoFilter ref="A1:O43" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O47" totalsRowShown="0">
+  <autoFilter ref="A1:O47" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -954,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2298,6 +2379,9 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>143</v>
+      </c>
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -2336,6 +2420,9 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>142</v>
+      </c>
       <c r="B41" t="s">
         <v>35</v>
       </c>
@@ -2437,27 +2524,137 @@
         <v>138</v>
       </c>
     </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>39</v>
+      </c>
+      <c r="I44" t="s">
+        <v>136</v>
+      </c>
+      <c r="J44">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="K44">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="L44">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="M44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" t="s">
+        <v>140</v>
+      </c>
+      <c r="J45">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="K45">
+        <v>0.625</v>
+      </c>
+      <c r="L45">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="M45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" t="s">
+        <v>39</v>
+      </c>
+      <c r="I46" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" t="s">
+        <v>39</v>
+      </c>
+      <c r="I47" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="9" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="8" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="15" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="7" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="6" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="13" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="5" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="4" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K43">
-    <cfRule type="top10" dxfId="3" priority="7" rank="2"/>
+  <conditionalFormatting sqref="K2:K47">
+    <cfRule type="top10" dxfId="9" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J43">
-    <cfRule type="top10" dxfId="2" priority="6" rank="2"/>
+  <conditionalFormatting sqref="J2:J47">
+    <cfRule type="top10" dxfId="8" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
test runs for avg before sampling
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39EBC47-576E-A84E-A3EE-1D4A04D45B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480639E-4DDC-B645-97C9-7747AEB1D654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="152">
   <si>
     <t>Model</t>
   </si>
@@ -161,9 +161,6 @@
     <t>weakly supervision</t>
   </si>
   <si>
-    <t>weakly supervision &amp; average before predictions</t>
-  </si>
-  <si>
     <t>Patients</t>
   </si>
   <si>
@@ -474,6 +471,27 @@
   </si>
   <si>
     <t>2023-03-10-1838_LogReg_minmax_avg.csv</t>
+  </si>
+  <si>
+    <t>0.640 (0.028)</t>
+  </si>
+  <si>
+    <t>standard scaling center data AFTER avg</t>
+  </si>
+  <si>
+    <t>0.648 (0.037)</t>
+  </si>
+  <si>
+    <t>min max scaling center data AFTER avg</t>
+  </si>
+  <si>
+    <t>0.634 (0.038)</t>
+  </si>
+  <si>
+    <t>0.639 (0.025)</t>
+  </si>
+  <si>
+    <t>weakly supervision &amp; avg before predictions</t>
   </si>
 </sst>
 </file>
@@ -540,27 +558,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -715,8 +713,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O47" totalsRowShown="0">
-  <autoFilter ref="A1:O47" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O51" totalsRowShown="0">
+  <autoFilter ref="A1:O51" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1035,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O47"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,8 +1045,8 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" customWidth="1"/>
     <col min="8" max="8" width="46.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="46.33203125" customWidth="1"/>
@@ -1084,16 +1082,16 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>79</v>
-      </c>
-      <c r="L1" t="s">
-        <v>80</v>
       </c>
       <c r="M1" t="s">
         <v>2</v>
@@ -1116,7 +1114,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1125,13 +1123,13 @@
         <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>
       </c>
       <c r="N2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O2">
         <v>0.6018</v>
@@ -1148,7 +1146,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -1157,13 +1155,13 @@
         <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M3" t="s">
         <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O3">
         <v>0.64300000000000002</v>
@@ -1180,7 +1178,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -1195,7 +1193,7 @@
         <v>17</v>
       </c>
       <c r="N4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O4">
         <v>0.61199999999999999</v>
@@ -1212,13 +1210,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -1227,7 +1225,7 @@
         <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O5">
         <v>0.58799999999999997</v>
@@ -1244,7 +1242,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -1253,13 +1251,13 @@
         <v>40</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O6">
         <v>0.53900000000000003</v>
@@ -1276,7 +1274,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -1285,13 +1283,13 @@
         <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O7">
         <v>0.57199999999999995</v>
@@ -1308,7 +1306,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -1317,13 +1315,13 @@
         <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -1346,7 +1344,7 @@
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J9">
         <v>0.57199999999999995</v>
@@ -1358,10 +1356,10 @@
         <v>0.60899999999999999</v>
       </c>
       <c r="M9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O9">
         <v>0.63100000000000001</v>
@@ -1387,13 +1385,13 @@
         <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O10">
         <v>0.58699999999999997</v>
@@ -1419,13 +1417,13 @@
         <v>40</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O11">
         <v>0.59899999999999998</v>
@@ -1451,7 +1449,7 @@
         <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J12">
         <v>0.628</v>
@@ -1463,10 +1461,10 @@
         <v>0.58699999999999997</v>
       </c>
       <c r="M12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O12">
         <v>0.60099999999999998</v>
@@ -1489,16 +1487,16 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="H13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O13">
         <v>0.60499999999999998</v>
@@ -1524,13 +1522,13 @@
         <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O14">
         <v>0.59099999999999997</v>
@@ -1556,7 +1554,7 @@
         <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J15">
         <v>0.63200000000000001</v>
@@ -1571,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O15">
         <v>0.59799999999999998</v>
@@ -1597,7 +1595,7 @@
         <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J16">
         <v>0.628</v>
@@ -1612,7 +1610,7 @@
         <v>4</v>
       </c>
       <c r="N16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O16">
         <v>0.59399999999999997</v>
@@ -1620,7 +1618,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
@@ -1653,7 +1651,7 @@
         <v>6</v>
       </c>
       <c r="N17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O17">
         <v>0.55800000000000005</v>
@@ -1661,7 +1659,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
@@ -1670,16 +1668,16 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
         <v>40</v>
       </c>
       <c r="I18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J18">
         <v>0.59699999999999998</v>
@@ -1688,7 +1686,7 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="N18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O18">
         <v>0.51600000000000001</v>
@@ -1696,7 +1694,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
@@ -1705,16 +1703,16 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
         <v>40</v>
       </c>
       <c r="I19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K19">
         <v>0.64700000000000002</v>
@@ -1723,7 +1721,7 @@
         <v>0.58699999999999997</v>
       </c>
       <c r="N19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O19">
         <v>0.51800000000000002</v>
@@ -1731,7 +1729,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
@@ -1740,16 +1738,16 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
         <v>40</v>
       </c>
       <c r="I20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J20">
         <v>0.61899999999999999</v>
@@ -1758,7 +1756,7 @@
         <v>0.58199999999999996</v>
       </c>
       <c r="N20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O20">
         <v>0.66600000000000004</v>
@@ -1766,7 +1764,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -1775,16 +1773,16 @@
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
         <v>40</v>
       </c>
       <c r="N21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O21">
         <v>0.64700000000000002</v>
@@ -1792,7 +1790,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
@@ -1801,16 +1799,16 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" t="s">
         <v>40</v>
       </c>
       <c r="N22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O22">
         <v>0.60299999999999998</v>
@@ -1818,7 +1816,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
@@ -1827,19 +1825,19 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" t="s">
         <v>40</v>
       </c>
       <c r="H23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O23">
         <v>0.64600000000000002</v>
@@ -1847,7 +1845,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
@@ -1856,16 +1854,16 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
         <v>40</v>
       </c>
       <c r="N24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O24">
         <v>0.624</v>
@@ -1873,7 +1871,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
         <v>35</v>
@@ -1882,22 +1880,22 @@
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F25" t="s">
         <v>40</v>
       </c>
       <c r="I25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L25">
         <v>0.60899999999999999</v>
       </c>
       <c r="N25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O25">
         <v>0.63100000000000001</v>
@@ -1905,7 +1903,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
@@ -1914,22 +1912,22 @@
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" t="s">
         <v>40</v>
       </c>
       <c r="I26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L26">
         <v>0.58599999999999997</v>
       </c>
       <c r="N26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O26">
         <v>0.60299999999999998</v>
@@ -1937,7 +1935,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
@@ -1946,16 +1944,16 @@
         <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
         <v>40</v>
       </c>
       <c r="I27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27">
         <v>0.56699999999999995</v>
@@ -1967,10 +1965,10 @@
         <v>0.61499999999999999</v>
       </c>
       <c r="M27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O27">
         <v>0.64400000000000002</v>
@@ -1978,7 +1976,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
         <v>38</v>
@@ -1987,16 +1985,16 @@
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
         <v>40</v>
       </c>
       <c r="I28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J28">
         <v>0.629</v>
@@ -2008,10 +2006,10 @@
         <v>0.60199999999999998</v>
       </c>
       <c r="M28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O28">
         <v>0.61199999999999999</v>
@@ -2019,7 +2017,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
@@ -2037,7 +2035,7 @@
         <v>39</v>
       </c>
       <c r="I29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J29">
         <v>0.60899999999999999</v>
@@ -2049,10 +2047,10 @@
         <v>0.628</v>
       </c>
       <c r="M29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O29">
         <v>0.58699999999999997</v>
@@ -2060,7 +2058,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
         <v>38</v>
@@ -2078,7 +2076,7 @@
         <v>39</v>
       </c>
       <c r="I30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J30">
         <v>0.57899999999999996</v>
@@ -2090,10 +2088,10 @@
         <v>0.62</v>
       </c>
       <c r="M30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O30">
         <v>0.63300000000000001</v>
@@ -2116,7 +2114,7 @@
         <v>39</v>
       </c>
       <c r="H31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J31">
         <v>0.60399999999999998</v>
@@ -2128,7 +2126,7 @@
         <v>0.68</v>
       </c>
       <c r="M31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -2157,12 +2155,12 @@
         <v>0.59899999999999998</v>
       </c>
       <c r="M32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -2186,12 +2184,12 @@
         <v>0.59699999999999998</v>
       </c>
       <c r="M33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -2215,12 +2213,12 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="M34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
@@ -2244,12 +2242,12 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="M35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -2273,12 +2271,12 @@
         <v>0.52900000000000003</v>
       </c>
       <c r="M36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
@@ -2296,13 +2294,13 @@
         <v>39</v>
       </c>
       <c r="H37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O37">
         <v>0.60699999999999998</v>
@@ -2310,7 +2308,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
@@ -2328,7 +2326,7 @@
         <v>39</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J38">
         <v>0.58299999999999996</v>
@@ -2340,10 +2338,10 @@
         <v>0.59799999999999998</v>
       </c>
       <c r="M38" t="s">
+        <v>124</v>
+      </c>
+      <c r="N38" t="s">
         <v>125</v>
-      </c>
-      <c r="N38" t="s">
-        <v>126</v>
       </c>
       <c r="O38">
         <v>0.60299999999999998</v>
@@ -2375,12 +2373,12 @@
         <v>0.63300000000000001</v>
       </c>
       <c r="M39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
@@ -2398,7 +2396,7 @@
         <v>39</v>
       </c>
       <c r="I40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J40">
         <v>0.61599999999999999</v>
@@ -2410,10 +2408,10 @@
         <v>0.63800000000000001</v>
       </c>
       <c r="M40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O40">
         <v>0.64900000000000002</v>
@@ -2421,7 +2419,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B41" t="s">
         <v>35</v>
@@ -2439,7 +2437,7 @@
         <v>39</v>
       </c>
       <c r="I41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J41">
         <v>0.64</v>
@@ -2451,10 +2449,10 @@
         <v>0.624</v>
       </c>
       <c r="M41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O41">
         <v>0.623</v>
@@ -2477,7 +2475,7 @@
         <v>39</v>
       </c>
       <c r="I42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J42">
         <v>0.59699999999999998</v>
@@ -2489,7 +2487,7 @@
         <v>0.61499999999999999</v>
       </c>
       <c r="M42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2509,7 +2507,7 @@
         <v>39</v>
       </c>
       <c r="I43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J43">
         <v>0.64</v>
@@ -2521,7 +2519,7 @@
         <v>0.66</v>
       </c>
       <c r="M43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2541,7 +2539,7 @@
         <v>39</v>
       </c>
       <c r="I44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J44">
         <v>0.60399999999999998</v>
@@ -2553,7 +2551,7 @@
         <v>0.61599999999999999</v>
       </c>
       <c r="M44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2573,7 +2571,7 @@
         <v>39</v>
       </c>
       <c r="I45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J45">
         <v>0.61099999999999999</v>
@@ -2585,12 +2583,12 @@
         <v>0.64800000000000002</v>
       </c>
       <c r="M45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B46" t="s">
         <v>38</v>
@@ -2608,12 +2606,12 @@
         <v>39</v>
       </c>
       <c r="I46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B47" t="s">
         <v>35</v>
@@ -2631,30 +2629,158 @@
         <v>39</v>
       </c>
       <c r="I47" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" t="s">
+        <v>39</v>
+      </c>
+      <c r="I48" t="s">
+        <v>146</v>
+      </c>
+      <c r="J48">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="K48">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="L48">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="M48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" t="s">
+        <v>39</v>
+      </c>
+      <c r="I49" t="s">
+        <v>148</v>
+      </c>
+      <c r="J49">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="K49">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="L49">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="M49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>39</v>
+      </c>
+      <c r="I50" t="s">
+        <v>146</v>
+      </c>
+      <c r="J50">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="K50">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="L50">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="M50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" t="s">
+        <v>39</v>
+      </c>
+      <c r="I51" t="s">
+        <v>148</v>
+      </c>
+      <c r="J51">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="K51">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="L51">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="M51" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="15" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="14" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="13" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="13" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="12" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="11" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="11" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="10" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K47">
-    <cfRule type="top10" dxfId="9" priority="7" rank="2"/>
+  <conditionalFormatting sqref="K2:K51">
+    <cfRule type="top10" dxfId="7" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J47">
-    <cfRule type="top10" dxfId="8" priority="6" rank="2"/>
+  <conditionalFormatting sqref="J2:J51">
+    <cfRule type="top10" dxfId="6" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
submitted minmax scaling RF & LogReg untuned
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C480639E-4DDC-B645-97C9-7747AEB1D654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376A60F4-7ABB-E449-A57C-27C9936701E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="154">
   <si>
     <t>Model</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>weakly supervision &amp; avg before predictions</t>
+  </si>
+  <si>
+    <t>March 11, 2023, 4:01 p.m.</t>
+  </si>
+  <si>
+    <t>March 11, 2023, 4:02 p.m.</t>
   </si>
 </sst>
 </file>
@@ -558,67 +564,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1035,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2608,6 +2554,12 @@
       <c r="I46" t="s">
         <v>135</v>
       </c>
+      <c r="N46" t="s">
+        <v>152</v>
+      </c>
+      <c r="O46">
+        <v>0.61299999999999999</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -2631,6 +2583,12 @@
       <c r="I47" t="s">
         <v>135</v>
       </c>
+      <c r="N47" t="s">
+        <v>153</v>
+      </c>
+      <c r="O47">
+        <v>0.59499999999999997</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
@@ -2763,24 +2721,24 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="13" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="12" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="7" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="11" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="10" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="5" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="9" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="8" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K51">
-    <cfRule type="top10" dxfId="7" priority="7" rank="2"/>
+    <cfRule type="top10" dxfId="1" priority="7" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J51">
-    <cfRule type="top10" dxfId="6" priority="6" rank="2"/>
+    <cfRule type="top10" dxfId="0" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
prepared tuned scaled RF submissions
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376A60F4-7ABB-E449-A57C-27C9936701E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F87CD70-6AAD-F446-B355-5103FB3481B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="160">
   <si>
     <t>Model</t>
   </si>
@@ -498,12 +498,33 @@
   </si>
   <si>
     <t>March 11, 2023, 4:02 p.m.</t>
+  </si>
+  <si>
+    <t>standard scaling center data before avg tuned</t>
+  </si>
+  <si>
+    <t>{'bootstrap': True,  'max_depth': 2, 'max_features': 0.5,  'max_samples': 0.8,  'min_samples_split': 10}</t>
+  </si>
+  <si>
+    <t>2023-03-11-1845_RF_Standard_avg_tuned.csv</t>
+  </si>
+  <si>
+    <t>minmax scaling center data before avg tuned</t>
+  </si>
+  <si>
+    <t>{'bootstrap': True, 'max_depth': 4,  'max_features': 1.0,  'max_samples': 0.7,  'min_samples_split': 10}</t>
+  </si>
+  <si>
+    <t>2023-03-11-1856_RF_MinMax_avg_tuned.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -557,14 +578,58 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -659,8 +724,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O51" totalsRowShown="0">
-  <autoFilter ref="A1:O51" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O53" totalsRowShown="0">
+  <autoFilter ref="A1:O53" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -979,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2622,7 +2687,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>35</v>
       </c>
@@ -2654,7 +2719,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>38</v>
       </c>
@@ -2686,7 +2751,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>38</v>
       </c>
@@ -2716,29 +2781,105 @@
       </c>
       <c r="M51" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" t="s">
+        <v>39</v>
+      </c>
+      <c r="H52" t="s">
+        <v>155</v>
+      </c>
+      <c r="I52" t="s">
+        <v>154</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.68883283650538896</v>
+      </c>
+      <c r="K52" s="2">
+        <v>0.70780051150895096</v>
+      </c>
+      <c r="L52" s="2">
+        <v>0.65485362095531596</v>
+      </c>
+      <c r="M52" s="3">
+        <v>0.68382898965655203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" t="s">
+        <v>158</v>
+      </c>
+      <c r="I53" t="s">
+        <v>157</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0.64939234120614497</v>
+      </c>
+      <c r="K53" s="2">
+        <v>0.74648337595907899</v>
+      </c>
+      <c r="L53" s="2">
+        <v>0.66358500256805297</v>
+      </c>
+      <c r="M53" s="3">
+        <v>0.68648690657776001</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="7" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="6" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="11" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="5" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="4" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="9" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="3" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K51">
-    <cfRule type="top10" dxfId="1" priority="7" rank="2"/>
+  <conditionalFormatting sqref="K2:K53">
+    <cfRule type="top10" dxfId="5" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J51">
-    <cfRule type="top10" dxfId="0" priority="6" rank="2"/>
+  <conditionalFormatting sqref="J2:J53">
+    <cfRule type="top10" dxfId="4" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added tuning results and results of using zoom level as numerical variable
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F87CD70-6AAD-F446-B355-5103FB3481B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868ADCF0-62D5-3E42-A1F0-EB4BBA74C8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="169">
   <si>
     <t>Model</t>
   </si>
@@ -516,6 +516,33 @@
   </si>
   <si>
     <t>2023-03-11-1856_RF_MinMax_avg_tuned.csv</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels</t>
+  </si>
+  <si>
+    <t>0.682 (0.053)</t>
+  </si>
+  <si>
+    <t>0.646 (0.037)</t>
+  </si>
+  <si>
+    <t>0.657 (0.039)</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling</t>
+  </si>
+  <si>
+    <t>0.668 (0.059)</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, minmax scaling</t>
+  </si>
+  <si>
+    <t>0.621 (0.022)</t>
+  </si>
+  <si>
+    <t>0.645 (0.052)</t>
   </si>
 </sst>
 </file>
@@ -523,7 +550,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -581,55 +608,15 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -724,8 +711,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O53" totalsRowShown="0">
-  <autoFilter ref="A1:O53" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O60" totalsRowShown="0">
+  <autoFilter ref="A1:O60" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1044,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="F30" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2687,7 +2674,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>35</v>
       </c>
@@ -2719,7 +2706,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>38</v>
       </c>
@@ -2751,7 +2738,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>38</v>
       </c>
@@ -2783,7 +2770,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>156</v>
       </c>
@@ -2820,8 +2807,11 @@
       <c r="M52" s="3">
         <v>0.68382898965655203</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="O52">
+        <v>0.60299999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>159</v>
       </c>
@@ -2857,29 +2847,256 @@
       </c>
       <c r="M53" s="3">
         <v>0.68648690657776001</v>
+      </c>
+      <c r="O53">
+        <v>0.63400000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" t="s">
+        <v>39</v>
+      </c>
+      <c r="I54" t="s">
+        <v>160</v>
+      </c>
+      <c r="J54">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K54">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="L54">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="M54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" t="s">
+        <v>39</v>
+      </c>
+      <c r="I55" t="s">
+        <v>160</v>
+      </c>
+      <c r="J55">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="K55">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="L55">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="M55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
+        <v>39</v>
+      </c>
+      <c r="I56" t="s">
+        <v>164</v>
+      </c>
+      <c r="J56">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="K56">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="L56">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="M56" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" t="s">
+        <v>39</v>
+      </c>
+      <c r="I57" t="s">
+        <v>166</v>
+      </c>
+      <c r="J57">
+        <v>0.6</v>
+      </c>
+      <c r="K57">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="L57">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="M57" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" t="s">
+        <v>39</v>
+      </c>
+      <c r="I58" t="s">
+        <v>160</v>
+      </c>
+      <c r="J58">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="K58">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="L58">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="M58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
+        <v>39</v>
+      </c>
+      <c r="I59" t="s">
+        <v>164</v>
+      </c>
+      <c r="J59">
+        <v>0.63</v>
+      </c>
+      <c r="K59">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="L59">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="M59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" t="s">
+        <v>39</v>
+      </c>
+      <c r="I60" t="s">
+        <v>166</v>
+      </c>
+      <c r="J60">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="K60">
+        <v>0.63</v>
+      </c>
+      <c r="L60">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="M60" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="11" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="10" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="7" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="9" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="8" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="5" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="7" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="6" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K53">
-    <cfRule type="top10" dxfId="5" priority="7" rank="2"/>
+  <conditionalFormatting sqref="K2:K60">
+    <cfRule type="top10" dxfId="1" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J53">
-    <cfRule type="top10" dxfId="4" priority="6" rank="2"/>
+  <conditionalFormatting sqref="J2:J60">
+    <cfRule type="top10" dxfId="0" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added option to one hot encode zoom levels
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868ADCF0-62D5-3E42-A1F0-EB4BBA74C8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8890E9F4-57AB-9449-A2EE-201EBBCD4EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="173">
   <si>
     <t>Model</t>
   </si>
@@ -543,6 +543,18 @@
   </si>
   <si>
     <t>0.645 (0.052)</t>
+  </si>
+  <si>
+    <t>incl. One hot Zoom levels</t>
+  </si>
+  <si>
+    <t>0.667 (0.053)</t>
+  </si>
+  <si>
+    <t>2023-03-12-1553_RF_zoom_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-12-1624_RF_zoomonehot_avg.csv</t>
   </si>
 </sst>
 </file>
@@ -711,8 +723,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O60" totalsRowShown="0">
-  <autoFilter ref="A1:O60" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O61" totalsRowShown="0">
+  <autoFilter ref="A1:O61" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1031,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O60"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F30" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2853,6 +2865,9 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>171</v>
+      </c>
       <c r="B54" t="s">
         <v>38</v>
       </c>
@@ -3074,6 +3089,41 @@
       </c>
       <c r="M60" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>172</v>
+      </c>
+      <c r="B61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" t="s">
+        <v>39</v>
+      </c>
+      <c r="I61" t="s">
+        <v>169</v>
+      </c>
+      <c r="J61">
+        <v>0.623</v>
+      </c>
+      <c r="K61">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="L61">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="M61" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3092,10 +3142,10 @@
   <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K60">
+  <conditionalFormatting sqref="K2:K61">
     <cfRule type="top10" dxfId="1" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J60">
+  <conditionalFormatting sqref="J2:J61">
     <cfRule type="top10" dxfId="0" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pos avg, standaridzation and zoom results
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145D769A-AC03-114C-8FBB-C57ADDB56274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9F1C33-9712-A941-B022-3F1999B403D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="192">
   <si>
     <t>Model</t>
   </si>
@@ -555,6 +555,63 @@
   </si>
   <si>
     <t>2023-03-12-1624_RF_zoomonehot_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-13-1610_RF_zoom_MinMax_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-13-1559_RF_zoom_Standard_avg.csv</t>
+  </si>
+  <si>
+    <t>0.659 (0.051)</t>
+  </si>
+  <si>
+    <t>2023-03-14-1833_Catboost_zoom_standard_avg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-14-1725_XGB_zoom_standard_avg.csv</t>
+  </si>
+  <si>
+    <t>March 13, 2023, 5:49 p.m.</t>
+  </si>
+  <si>
+    <t>March 14, 2023, 5:52 p.m.</t>
+  </si>
+  <si>
+    <t>March 12, 2023, 5:33 p.m.</t>
+  </si>
+  <si>
+    <t>March 13, 2023, 5:48 p.m.</t>
+  </si>
+  <si>
+    <t>0.657 (0.042)</t>
+  </si>
+  <si>
+    <t>pos average</t>
+  </si>
+  <si>
+    <t>0.666 (0.037)</t>
+  </si>
+  <si>
+    <t>0.638 (0.029)</t>
+  </si>
+  <si>
+    <t>0.623 (0.042)</t>
+  </si>
+  <si>
+    <t>0.661 (0.032)</t>
+  </si>
+  <si>
+    <t>0.680 (0.028)</t>
+  </si>
+  <si>
+    <t>March 15, 2023, 5:54 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-15-1552_Catboost_zoom_standard_posavg.csv</t>
+  </si>
+  <si>
+    <t>2023-03-15-1555_RF_zoom_standard_posavg.csv</t>
   </si>
 </sst>
 </file>
@@ -586,12 +643,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -617,13 +680,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -723,8 +787,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O61" totalsRowShown="0">
-  <autoFilter ref="A1:O61" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O69" totalsRowShown="0">
+  <autoFilter ref="A1:O69" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1043,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H30" workbookViewId="0">
-      <selection activeCell="O55" sqref="O55"/>
+    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2935,6 +2999,9 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>174</v>
+      </c>
       <c r="B56" t="s">
         <v>38</v>
       </c>
@@ -2965,8 +3032,17 @@
       <c r="M56" t="s">
         <v>163</v>
       </c>
+      <c r="N56" t="s">
+        <v>178</v>
+      </c>
+      <c r="O56">
+        <v>0.67900000000000005</v>
+      </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>173</v>
+      </c>
       <c r="B57" t="s">
         <v>38</v>
       </c>
@@ -2996,6 +3072,12 @@
       </c>
       <c r="M57" t="s">
         <v>165</v>
+      </c>
+      <c r="N57" t="s">
+        <v>181</v>
+      </c>
+      <c r="O57">
+        <v>0.63500000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -3031,6 +3113,9 @@
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>177</v>
+      </c>
       <c r="B59" t="s">
         <v>37</v>
       </c>
@@ -3060,6 +3145,12 @@
       </c>
       <c r="M59" t="s">
         <v>168</v>
+      </c>
+      <c r="N59" t="s">
+        <v>179</v>
+      </c>
+      <c r="O59">
+        <v>0.58499999999999996</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
@@ -3128,8 +3219,262 @@
       <c r="M61" t="s">
         <v>170</v>
       </c>
+      <c r="N61" t="s">
+        <v>180</v>
+      </c>
       <c r="O61">
         <v>0.61180000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>176</v>
+      </c>
+      <c r="B62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" t="s">
+        <v>39</v>
+      </c>
+      <c r="I62" t="s">
+        <v>164</v>
+      </c>
+      <c r="J62">
+        <v>0.64</v>
+      </c>
+      <c r="K62">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="L62">
+        <v>0.61</v>
+      </c>
+      <c r="M62" t="s">
+        <v>175</v>
+      </c>
+      <c r="N62" t="s">
+        <v>179</v>
+      </c>
+      <c r="O62">
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" t="s">
+        <v>183</v>
+      </c>
+      <c r="I63" t="s">
+        <v>160</v>
+      </c>
+      <c r="J63">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="K63">
+        <v>0.71</v>
+      </c>
+      <c r="L63">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="M63" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>191</v>
+      </c>
+      <c r="B64" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" t="s">
+        <v>183</v>
+      </c>
+      <c r="I64" t="s">
+        <v>164</v>
+      </c>
+      <c r="J64">
+        <v>0.624</v>
+      </c>
+      <c r="K64">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="L64">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="M64" t="s">
+        <v>185</v>
+      </c>
+      <c r="N64" t="s">
+        <v>189</v>
+      </c>
+      <c r="O64">
+        <v>0.629</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" t="s">
+        <v>183</v>
+      </c>
+      <c r="I65" t="s">
+        <v>166</v>
+      </c>
+      <c r="J65">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="K65">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="L65">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="M65" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" t="s">
+        <v>183</v>
+      </c>
+      <c r="I66" t="s">
+        <v>160</v>
+      </c>
+      <c r="J66">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K66">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="L66">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="M66" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" t="s">
+        <v>115</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" t="s">
+        <v>183</v>
+      </c>
+      <c r="I67" t="s">
+        <v>164</v>
+      </c>
+      <c r="J67">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="K67">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="L67">
+        <v>0.67</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="N67" t="s">
+        <v>189</v>
+      </c>
+      <c r="O67">
+        <v>0.65800000000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" t="s">
+        <v>183</v>
+      </c>
+      <c r="I68" t="s">
+        <v>166</v>
+      </c>
+      <c r="J68">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K68">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="L68">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="M68" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3148,10 +3493,10 @@
   <conditionalFormatting sqref="J1:J1048576">
     <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K61">
+  <conditionalFormatting sqref="K2:K69">
     <cfRule type="top10" dxfId="1" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J61">
+  <conditionalFormatting sqref="J2:J69">
     <cfRule type="top10" dxfId="0" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
drop dupes after scaling
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9F1C33-9712-A941-B022-3F1999B403D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2B4E7A-6E71-1A4F-BF26-B1A61FD06C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="205">
   <si>
     <t>Model</t>
   </si>
@@ -612,6 +612,45 @@
   </si>
   <si>
     <t>2023-03-15-1555_RF_zoom_standard_posavg.csv</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling, keep dupes first</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling, keep dupes diverse zoom</t>
+  </si>
+  <si>
+    <t>0.679 (0.040)</t>
+  </si>
+  <si>
+    <t>0.658 (0.022)</t>
+  </si>
+  <si>
+    <t>0.644 (0.030)</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling, keep dupes last</t>
+  </si>
+  <si>
+    <t>0.681 (0.053)</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling, keep dupes all 16</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling, keep 15/16</t>
+  </si>
+  <si>
+    <t>0.686 (0.042)</t>
+  </si>
+  <si>
+    <t>March 18, 2023, 5:53 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-18-1852_Catboost_zoom_pos_avg_dup_16.csv</t>
+  </si>
+  <si>
+    <t>0.617 (0.023)</t>
   </si>
 </sst>
 </file>
@@ -692,7 +731,107 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -787,8 +926,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O69" totalsRowShown="0">
-  <autoFilter ref="A1:O69" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O74" totalsRowShown="0">
+  <autoFilter ref="A1:O74" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1107,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="L63" sqref="L63"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3477,27 +3616,228 @@
         <v>187</v>
       </c>
     </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" t="s">
+        <v>183</v>
+      </c>
+      <c r="I69" t="s">
+        <v>192</v>
+      </c>
+      <c r="J69">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="K69">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="L69">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="M69" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>115</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" t="s">
+        <v>183</v>
+      </c>
+      <c r="I70" t="s">
+        <v>197</v>
+      </c>
+      <c r="J70">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="K70">
+        <v>0.73</v>
+      </c>
+      <c r="L70">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="M70" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" t="s">
+        <v>183</v>
+      </c>
+      <c r="I71" t="s">
+        <v>193</v>
+      </c>
+      <c r="J71">
+        <v>0.66</v>
+      </c>
+      <c r="K71">
+        <v>0.67</v>
+      </c>
+      <c r="L71">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="M71" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" t="s">
+        <v>183</v>
+      </c>
+      <c r="I72" t="s">
+        <v>199</v>
+      </c>
+      <c r="J72">
+        <v>0.622</v>
+      </c>
+      <c r="K72">
+        <v>0.75</v>
+      </c>
+      <c r="L72">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="M72" t="s">
+        <v>198</v>
+      </c>
+      <c r="N72" t="s">
+        <v>202</v>
+      </c>
+      <c r="O72">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>203</v>
+      </c>
+      <c r="B73" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" t="s">
+        <v>183</v>
+      </c>
+      <c r="I73" t="s">
+        <v>200</v>
+      </c>
+      <c r="J73">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="K73">
+        <v>0.745</v>
+      </c>
+      <c r="L73">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="M73" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" t="s">
+        <v>183</v>
+      </c>
+      <c r="I74" t="s">
+        <v>199</v>
+      </c>
+      <c r="J74">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="K74">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="L74">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="M74" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="7" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="6" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="17" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="5" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="4" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="15" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="3" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K69">
-    <cfRule type="top10" dxfId="1" priority="7" rank="2"/>
+  <conditionalFormatting sqref="K2:K74">
+    <cfRule type="top10" dxfId="11" priority="7" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J69">
-    <cfRule type="top10" dxfId="0" priority="6" rank="2"/>
+  <conditionalFormatting sqref="J2:J74">
+    <cfRule type="top10" dxfId="10" priority="6" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
filtering for dupes before scaling
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2B4E7A-6E71-1A4F-BF26-B1A61FD06C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E189030-FBF2-2540-B89C-B6D50A88E0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="211">
   <si>
     <t>Model</t>
   </si>
@@ -647,10 +647,28 @@
     <t>March 18, 2023, 5:53 p.m.</t>
   </si>
   <si>
-    <t>2023-03-18-1852_Catboost_zoom_pos_avg_dup_16.csv</t>
-  </si>
-  <si>
     <t>0.617 (0.023)</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling, keep dupes diverse zoom before scaling</t>
+  </si>
+  <si>
+    <t>incl. Zoom levels, standard scaling, keep dupes all 16 before scaling</t>
+  </si>
+  <si>
+    <t>0.645 (0.024)</t>
+  </si>
+  <si>
+    <t>0.683 (0.058)</t>
+  </si>
+  <si>
+    <t>2023-03-18-1852_Catboost_zoom_pos_avg_standard_dup_16.csv</t>
+  </si>
+  <si>
+    <t>March 18, 2023, 6:35 p.m.</t>
+  </si>
+  <si>
+    <t>0.632 (0.063)</t>
   </si>
 </sst>
 </file>
@@ -682,18 +700,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -719,19 +731,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -764,51 +775,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -912,6 +883,26 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -926,8 +917,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O74" totalsRowShown="0">
-  <autoFilter ref="A1:O74" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O77" totalsRowShown="0">
+  <autoFilter ref="A1:O77" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1246,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O74"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" topLeftCell="F44" workbookViewId="0">
+      <selection activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3574,7 +3565,7 @@
       <c r="L67">
         <v>0.67</v>
       </c>
-      <c r="M67" s="4" t="s">
+      <c r="M67" t="s">
         <v>188</v>
       </c>
       <c r="N67" t="s">
@@ -3752,7 +3743,7 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B73" t="s">
         <v>115</v>
@@ -3814,30 +3805,141 @@
         <v>0.63100000000000001</v>
       </c>
       <c r="M74" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>115</v>
+      </c>
+      <c r="C75" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" t="s">
+        <v>183</v>
+      </c>
+      <c r="I75" t="s">
         <v>204</v>
+      </c>
+      <c r="J75">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K75">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="L75">
+        <v>0.623</v>
+      </c>
+      <c r="M75" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>208</v>
+      </c>
+      <c r="B76" t="s">
+        <v>115</v>
+      </c>
+      <c r="C76" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" t="s">
+        <v>183</v>
+      </c>
+      <c r="I76" t="s">
+        <v>205</v>
+      </c>
+      <c r="J76">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="K76">
+        <v>0.753</v>
+      </c>
+      <c r="L76">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="M76" t="s">
+        <v>207</v>
+      </c>
+      <c r="N76" t="s">
+        <v>209</v>
+      </c>
+      <c r="O76">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" t="s">
+        <v>39</v>
+      </c>
+      <c r="I77" t="s">
+        <v>205</v>
+      </c>
+      <c r="J77">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="K77">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="L77">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="M77" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="17" priority="4" rank="1"/>
-    <cfRule type="top10" dxfId="16" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="13" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="11" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="15" priority="3" rank="1"/>
-    <cfRule type="top10" dxfId="14" priority="8" rank="2"/>
+    <cfRule type="top10" dxfId="11" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="10" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="13" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="12" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K74">
-    <cfRule type="top10" dxfId="11" priority="7" rank="2"/>
+  <conditionalFormatting sqref="K2:K77">
+    <cfRule type="top10" dxfId="7" priority="9" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J74">
-    <cfRule type="top10" dxfId="10" priority="6" rank="2"/>
+  <conditionalFormatting sqref="J2:J77">
+    <cfRule type="top10" dxfId="6" priority="8" rank="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M67">
+    <cfRule type="top10" dxfId="3" priority="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M67">
+    <cfRule type="top10" dxfId="2" priority="2" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
submission with zoom based scaling
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E189030-FBF2-2540-B89C-B6D50A88E0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFC0DAE-3509-4C41-839E-916BA6400E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="239">
   <si>
     <t>Model</t>
   </si>
@@ -669,6 +669,90 @@
   </si>
   <si>
     <t>0.632 (0.063)</t>
+  </si>
+  <si>
+    <t>zoom, dupes low sample ID, standard scaling</t>
+  </si>
+  <si>
+    <t>zoom, dupes high sample ID, standard scaling</t>
+  </si>
+  <si>
+    <t>0.669 (0.041)</t>
+  </si>
+  <si>
+    <t>0.660 (0.026)</t>
+  </si>
+  <si>
+    <t>zoom, dupes diverse &amp; high sample ID, standard scaling</t>
+  </si>
+  <si>
+    <t>zoom, dupes 16 &amp; low sample ID, standard scaling</t>
+  </si>
+  <si>
+    <t>zoom, dupes low &amp; low sample ID, standard scaling</t>
+  </si>
+  <si>
+    <t>0.647 (0.041)</t>
+  </si>
+  <si>
+    <t>0.681 (0.039)</t>
+  </si>
+  <si>
+    <t>0.673 (0.038)</t>
+  </si>
+  <si>
+    <t>zoom, dupes high &amp; high sample ID, standard scaling</t>
+  </si>
+  <si>
+    <t>0.644 (0.042)</t>
+  </si>
+  <si>
+    <t>zoom, standard scaling per zoom</t>
+  </si>
+  <si>
+    <t>0.664 (0.041)</t>
+  </si>
+  <si>
+    <t>zoom, MinMax scaling per zoom</t>
+  </si>
+  <si>
+    <t>0.642 (0.040)</t>
+  </si>
+  <si>
+    <t>0.659 (0.002)</t>
+  </si>
+  <si>
+    <t>0.641 (0.039)</t>
+  </si>
+  <si>
+    <t>March 20, 2023, 10:01 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-20-2300_Catboost_zoom_MinMax_per_zoom.csv</t>
+  </si>
+  <si>
+    <t>zoom,  dupes low &amp; low sample ID, MinMax scaling per zoom</t>
+  </si>
+  <si>
+    <t>zoom, dupes high &amp; high sample ID, MinMax scaling per zoom</t>
+  </si>
+  <si>
+    <t>0.665 (0.024)</t>
+  </si>
+  <si>
+    <t>0.653 (0.024)</t>
+  </si>
+  <si>
+    <t>{"l2_leaf_reg": 2}</t>
+  </si>
+  <si>
+    <t>0.668 (0.013)</t>
+  </si>
+  <si>
+    <t>0.666 (0.008)</t>
+  </si>
+  <si>
+    <t>{"l2_leaf_reg": 5}</t>
   </si>
 </sst>
 </file>
@@ -731,18 +815,161 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -780,26 +1007,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -883,26 +1090,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -917,8 +1104,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O77" totalsRowShown="0">
-  <autoFilter ref="A1:O77" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O91" totalsRowShown="0">
+  <autoFilter ref="A1:O91" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -1237,10 +1424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F44" workbookViewId="0">
-      <selection activeCell="L78" sqref="L78"/>
+    <sheetView tabSelected="1" topLeftCell="H56" workbookViewId="0">
+      <selection activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3790,7 +3977,7 @@
         <v>19</v>
       </c>
       <c r="F74" t="s">
-        <v>183</v>
+        <v>39</v>
       </c>
       <c r="I74" t="s">
         <v>199</v>
@@ -3913,33 +4100,496 @@
         <v>210</v>
       </c>
     </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B78" t="s">
+        <v>115</v>
+      </c>
+      <c r="C78" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" t="s">
+        <v>183</v>
+      </c>
+      <c r="I78" t="s">
+        <v>212</v>
+      </c>
+      <c r="J78">
+        <v>0.625</v>
+      </c>
+      <c r="K78">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="L78">
+        <v>0.66</v>
+      </c>
+      <c r="M78" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>115</v>
+      </c>
+      <c r="C79" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" t="s">
+        <v>183</v>
+      </c>
+      <c r="I79" t="s">
+        <v>211</v>
+      </c>
+      <c r="J79">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="K79">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="L79">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="M79" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" t="s">
+        <v>183</v>
+      </c>
+      <c r="I80" t="s">
+        <v>215</v>
+      </c>
+      <c r="J80">
+        <v>0.628</v>
+      </c>
+      <c r="K80">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="L80">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="M80" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>115</v>
+      </c>
+      <c r="C81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" t="s">
+        <v>183</v>
+      </c>
+      <c r="I81" t="s">
+        <v>216</v>
+      </c>
+      <c r="J81">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="K81">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="L81">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="M81" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B82" t="s">
+        <v>115</v>
+      </c>
+      <c r="C82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" t="s">
+        <v>183</v>
+      </c>
+      <c r="I82" t="s">
+        <v>217</v>
+      </c>
+      <c r="J82">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="K82">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="L82">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="M82" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B83" t="s">
+        <v>115</v>
+      </c>
+      <c r="C83" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" t="s">
+        <v>19</v>
+      </c>
+      <c r="F83" t="s">
+        <v>183</v>
+      </c>
+      <c r="I83" t="s">
+        <v>221</v>
+      </c>
+      <c r="J83">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="K83">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="L83">
+        <v>0.629</v>
+      </c>
+      <c r="M83" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>115</v>
+      </c>
+      <c r="C84" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" t="s">
+        <v>183</v>
+      </c>
+      <c r="I84" t="s">
+        <v>223</v>
+      </c>
+      <c r="J84">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="K84">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="L84">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="M84" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" t="s">
+        <v>39</v>
+      </c>
+      <c r="I85" t="s">
+        <v>223</v>
+      </c>
+      <c r="J85">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="K85">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="L85">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="M85" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>230</v>
+      </c>
+      <c r="B86" t="s">
+        <v>115</v>
+      </c>
+      <c r="C86" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" t="s">
+        <v>183</v>
+      </c>
+      <c r="I86" t="s">
+        <v>225</v>
+      </c>
+      <c r="J86">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="K86">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="L86">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="M86" t="s">
+        <v>227</v>
+      </c>
+      <c r="N86" t="s">
+        <v>229</v>
+      </c>
+      <c r="O86">
+        <v>0.64300000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>115</v>
+      </c>
+      <c r="C87" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" t="s">
+        <v>39</v>
+      </c>
+      <c r="I87" t="s">
+        <v>225</v>
+      </c>
+      <c r="J87">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="K87">
+        <v>0.69</v>
+      </c>
+      <c r="L87">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="M87" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>115</v>
+      </c>
+      <c r="C88" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" t="s">
+        <v>183</v>
+      </c>
+      <c r="I88" t="s">
+        <v>231</v>
+      </c>
+      <c r="J88">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="K88">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="L88">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="M88" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" t="s">
+        <v>19</v>
+      </c>
+      <c r="F89" t="s">
+        <v>183</v>
+      </c>
+      <c r="I89" t="s">
+        <v>232</v>
+      </c>
+      <c r="J89">
+        <v>0.628</v>
+      </c>
+      <c r="K89">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="L89">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="M89" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>115</v>
+      </c>
+      <c r="C90" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" t="s">
+        <v>19</v>
+      </c>
+      <c r="F90" t="s">
+        <v>183</v>
+      </c>
+      <c r="H90" t="s">
+        <v>235</v>
+      </c>
+      <c r="I90" t="s">
+        <v>225</v>
+      </c>
+      <c r="J90">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="K90">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="L90">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="M90" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>115</v>
+      </c>
+      <c r="C91" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" t="s">
+        <v>19</v>
+      </c>
+      <c r="F91" t="s">
+        <v>183</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="I91" t="s">
+        <v>225</v>
+      </c>
+      <c r="J91">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="K91">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="L91">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="M91" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="13" priority="6" rank="1"/>
-    <cfRule type="top10" dxfId="12" priority="11" rank="2"/>
+    <cfRule type="top10" dxfId="25" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="11" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="11" priority="5" rank="1"/>
-    <cfRule type="top10" dxfId="10" priority="10" rank="2"/>
+    <cfRule type="top10" dxfId="23" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="10" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="9" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="8" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K77">
-    <cfRule type="top10" dxfId="7" priority="9" rank="2"/>
+  <conditionalFormatting sqref="K2:K91">
+    <cfRule type="top10" dxfId="19" priority="9" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J77">
-    <cfRule type="top10" dxfId="6" priority="8" rank="2"/>
+  <conditionalFormatting sqref="J2:J91">
+    <cfRule type="top10" dxfId="18" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="3" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="2" priority="2" rank="2"/>
+    <cfRule type="top10" dxfId="16" priority="2" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
finalised dupes drop with manually selected drop list
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFC0DAE-3509-4C41-839E-916BA6400E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E848F117-23AB-2C40-B9C9-AC0523764EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="323">
   <si>
     <t>Model</t>
   </si>
@@ -753,6 +753,730 @@
   </si>
   <si>
     <t>{"l2_leaf_reg": 5}</t>
+  </si>
+  <si>
+    <t>zoom, manual dupes, standard scaling</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', 
+            'ID_083.npy', 'ID_102.npy', 'ID_111.npy', 'ID_117.npy',
+            'ID_130.npy', 'ID_132.npy', 'ID_161.npy', 'ID_233.npy',
+            'ID_243.npy', 'ID_252.npy', 'ID_257.npy', 'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>Drop List</t>
+  </si>
+  <si>
+    <t>0.682 (0.040)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', 
+            'ID_081.npy', 
+            'ID_102.npy', 'ID_111.npy', 'ID_117.npy',
+            'ID_130.npy', 'ID_132.npy', 'ID_161.npy', 'ID_233.npy',
+            'ID_243.npy', 'ID_252.npy', 'ID_257.npy', 'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', 
+            'ID_083.npy', 'ID_073.npy',
+            'ID_111.npy', 'ID_117.npy',
+            'ID_130.npy', 'ID_132.npy', 'ID_161.npy', 'ID_233.npy',
+            'ID_243.npy', 'ID_252.npy', 'ID_257.npy', 'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.672 (0.045)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy',
+            'ID_130.npy', 'ID_132.npy', 'ID_161.npy', 'ID_233.npy',
+            'ID_243.npy', 'ID_252.npy', 'ID_257.npy', 'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.677 (0.045)</t>
+  </si>
+  <si>
+    <t>0.689 (0.041)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_203.npy', # 'ID_233.npy',
+            'ID_161.npy', 
+            'ID_243.npy', 'ID_252.npy', 'ID_257.npy', 'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.683 (0.039)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_182.npy', # 'ID_243.npy',
+            'ID_252.npy', 'ID_257.npy', 'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.682 (0.044)</t>
+  </si>
+  <si>
+    <t>0.698 (0.046)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_141.npy', # 'ID_257.npy', 
+            'ID_260.npy',
+            'ID_272.npy', 'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_025.npy', # 'ID_272.npy', 
+            'ID_276.npy', 'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.688 (0.049)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.688 (0.048)</t>
+  </si>
+  <si>
+    <t>0.704 (0.051)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_059.npy', # 'ID_278.npy', 
+            'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.696 (0.054)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_259.npy', # 'ID_279.npy',
+            'ID_296.npy', 'ID_316.npy', 'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>March 21, 2023, 10:32 a.m.</t>
+  </si>
+  <si>
+    <t>2023-03-21-1131_Catboost_zoom_dupes_manual_standard.csv</t>
+  </si>
+  <si>
+    <t>0.697 (0.052)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_167.npy', #'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.682 (0.047)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_287.npy', # 'ID_328.npy',
+            'ID_334.npy', 'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.694 (0.049)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_057.npy', # 'ID_334.npy', 
+            'ID_353.npy', 'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.704 (0.050)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_050.npy', # 'ID_355.npy', 
+            'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.695 (0.059)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_238.npy', # 'ID_358.npy',
+            'ID_371.npy', 'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_097.npy', # 'ID_371.npy', 
+            'ID_411.npy', 'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.687 (0.061)</t>
+  </si>
+  <si>
+    <t>0.684 (0.054)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_168.npy', #'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.692 (0.057)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_348.npy', # 'ID_437.npy', 
+            'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_248.npy', # 'ID_440.npy',
+            'ID_455.npy', 'ID_460.npy', 'ID_461.npy', 'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.695 (0.061)</t>
+  </si>
+  <si>
+    <t>0.691 (0.052)</t>
+  </si>
+  <si>
+    <t>0.694 (0.054)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_128.npy', # 'ID_465.npy', 
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_020.npy', # 'ID_461.npy', 
+            'ID_465.npy',
+            'ID_481.npy', 'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.699 (0.060)</t>
+  </si>
+  <si>
+    <t>0.686 (0.058)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_465.npy', 'ID_398.npy', # 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_465.npy', 'ID_481.npy', 
+            'ID_468.npy', # 'ID_484.npy', 
+            'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.690 (0.058)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_293.npy'] # 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.700 (0.053)</t>
+  </si>
+  <si>
+    <t>0.692 (0.054)</t>
+  </si>
+  <si>
+    <t>['ID_196.npy',  # 'ID_014.npy', 
+             'ID_028.npy', 'ID_052.npy', 'ID_074.npy', # 'ID_082.npy'
+            'ID_083.npy', 'ID_102.npy', 'ID_094.npy', # 'ID_111.npy'
+            'ID_117.npy', 'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', # 'ID_252.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', # 'ID_276.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', # 'ID_353.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 
+            'ID_470.npy',  # 'ID_028.npy', 
+            'ID_052.npy', # 'ID_325.npy', # 
+            'ID_117.npy', # 'ID_005.npy', # 
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 'ID_094.npy', 
+            'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.694 (0.053)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 
+            'ID_325.npy', # 'ID_052.npy'
+            'ID_117.npy', # 'ID_005.npy', # 
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 'ID_094.npy', 
+            'ID_130.npy', 'ID_132.npy', 'ID_233.npy',
+            'ID_161.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_260.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.688 (0.050)</t>
+  </si>
+  <si>
+    <t>0.687 (0.055)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy',
+            'ID_005.npy', # 'ID_117.npy',
+            'ID_130.npy',
+            'ID_132.npy', 'ID_233.npy', # 'ID_203.npy', # 
+            'ID_161.npy',
+            'ID_260.npy',
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 'ID_094.npy', 
+            'ID_243.npy', 'ID_055.npy', 'ID_257.npy', 
+            'ID_272.npy', 'ID_274.npy', 'ID_278.npy', 
+            'ID_279.npy', 'ID_296.npy', 'ID_316.npy', 
+            'ID_324.npy', 'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_355.npy', 'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_440.npy', 'ID_455.npy', 'ID_460.npy', 
+            'ID_461.npy', 'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 'ID_117.npy',
+            'ID_251.npy', # 'ID_130.npy',
+            'ID_132.npy', 'ID_233.npy', # 'ID_203.npy', # 
+            'ID_161.npy',
+            'ID_260.npy',
+            'ID_296.npy',
+            'ID_324.npy',
+            'ID_355.npy', 
+            'ID_440.npy', 
+            'ID_455.npy',
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.694 (0.051)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy',
+             'ID_203.npy', 'ID_233.npy', #  # 'ID_132.npy',
+            'ID_161.npy', # 'ID_474.npy'
+            'ID_260.npy', # 'ID_312.npy'
+            'ID_296.npy', # 'ID_436.npy'
+            'ID_324.npy', # 'ID_192.npy'
+            'ID_355.npy', # 'ID_050.npy'
+            'ID_440.npy', 
+            'ID_455.npy',
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.691 (0.049)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy',
+             'ID_132.npy', 'ID_233.npy',
+             'ID_474.npy', # 'ID_161.npy',
+            'ID_260.npy', # 'ID_312.npy'
+            'ID_296.npy', # 'ID_436.npy'
+            'ID_324.npy', # 'ID_192.npy'
+            'ID_355.npy', # 'ID_050.npy'
+            'ID_440.npy', # 'ID_248.npy'
+            'ID_455.npy', # 'ID_170.npy'
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.680 (0.061)</t>
+  </si>
+  <si>
+    <t>0.700 (0.046)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy',
+             'ID_132.npy', 'ID_233.npy',
+             'ID_474.npy',
+            'ID_312.npy', # 'ID_260.npy', # 
+            'ID_296.npy', # 'ID_436.npy'
+            'ID_324.npy', # 'ID_192.npy'
+            'ID_355.npy', # 'ID_050.npy'
+            'ID_440.npy', # 'ID_248.npy'
+            'ID_455.npy', # 'ID_170.npy'
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.683 (0.055)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy', 'ID_132.npy', 
+             'ID_233.npy', 'ID_474.npy', 'ID_260.npy', 
+            'ID_436.npy', # 'ID_296.npy', #
+            'ID_324.npy', # 'ID_192.npy'
+            'ID_355.npy', # 'ID_050.npy'
+            'ID_440.npy', # 'ID_248.npy'
+            'ID_455.npy', # 'ID_170.npy'
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy', 'ID_132.npy', 
+             'ID_233.npy', 'ID_474.npy', 'ID_260.npy', 
+            'ID_296.npy', 
+            'ID_192.npy', # 'ID_324.npy', # 
+            'ID_355.npy', # 'ID_050.npy'
+            'ID_440.npy', # 'ID_248.npy'
+            'ID_455.npy', # 'ID_170.npy'
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.686 (0.055)</t>
+  </si>
+  <si>
+    <t>0.680 (0.046)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy', 'ID_132.npy', 
+             'ID_233.npy', 'ID_474.npy', 'ID_260.npy', 
+            'ID_296.npy', 'ID_324.npy',
+            'ID_050.npy', # 'ID_355.npy', # 
+            'ID_440.npy', # 'ID_248.npy'
+            'ID_455.npy', # 'ID_170.npy'
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy', 'ID_132.npy', 
+             'ID_233.npy', 'ID_474.npy', 'ID_260.npy', 
+            'ID_296.npy', 'ID_324.npy', 'ID_355.npy', 
+            'ID_248.npy', # 'ID_440.npy', # 
+            'ID_455.npy', # 'ID_170.npy'
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.691 (0.057)</t>
+  </si>
+  <si>
+    <t>0.695 (0.047)</t>
+  </si>
+  <si>
+    <t>['ID_014.npy', 'ID_028.npy', 'ID_052.npy', 
+             'ID_117.npy','ID_130.npy', 'ID_132.npy', 
+             'ID_233.npy', 'ID_474.npy', 'ID_260.npy', 
+            'ID_296.npy', 'ID_324.npy', 'ID_355.npy', 
+            'ID_440.npy',
+            'ID_170.npy', # 'ID_455.npy', # 
+            'ID_074.npy', 'ID_083.npy', 'ID_102.npy', 
+            'ID_094.npy', 'ID_243.npy', 'ID_055.npy', 
+            'ID_257.npy', 'ID_272.npy', 'ID_274.npy', 
+            'ID_278.npy', 'ID_279.npy', 'ID_316.npy', 
+            'ID_328.npy', 'ID_334.npy', 'ID_099.npy', 
+            'ID_358.npy', 'ID_371.npy', 'ID_411.npy', 
+            'ID_437.npy', 'ID_460.npy', 'ID_461.npy', 
+            'ID_465.npy', 'ID_481.npy', 
+            'ID_484.npy', 'ID_491.npy']</t>
+  </si>
+  <si>
+    <t>0.687 (0.056)</t>
   </si>
 </sst>
 </file>
@@ -784,12 +1508,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -815,7 +1545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -825,111 +1555,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1104,9 +1737,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:O91" totalsRowShown="0">
-  <autoFilter ref="A1:O91" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P134" totalsRowShown="0">
+  <autoFilter ref="A1:P134" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
     <tableColumn id="3" xr3:uid="{A38F4111-BA96-B34B-ABA6-3C86C9C9AFB0}" name="Data"/>
@@ -1122,6 +1755,7 @@
     <tableColumn id="12" xr3:uid="{4D8DB703-25AA-904E-8326-928036B74DBD}" name="Average Val AUC"/>
     <tableColumn id="13" xr3:uid="{F3337869-98B7-A24C-BF08-7BB0004966EC}" name="Hand in"/>
     <tableColumn id="14" xr3:uid="{B25C33D3-3F61-A54D-AC75-1293A620D8B4}" name="Test AUC"/>
+    <tableColumn id="16" xr3:uid="{FB5D958C-184B-FD46-BAE8-A8FC0C472DF5}" name="Drop List"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1424,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:O91"/>
+  <dimension ref="A1:P132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H56" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView tabSelected="1" topLeftCell="F105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1445,9 +2079,10 @@
     <col min="13" max="13" width="17.5" customWidth="1"/>
     <col min="14" max="14" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1493,8 +2128,11 @@
       <c r="O1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1526,7 +2164,7 @@
         <v>0.6018</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1558,7 +2196,7 @@
         <v>0.64300000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1590,7 +2228,7 @@
         <v>0.61199999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1622,7 +2260,7 @@
         <v>0.58799999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1654,7 +2292,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1686,7 +2324,7 @@
         <v>0.57199999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1715,7 +2353,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1756,7 +2394,7 @@
         <v>0.63100000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1788,7 +2426,7 @@
         <v>0.58699999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1820,7 +2458,7 @@
         <v>0.59899999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1861,7 +2499,7 @@
         <v>0.60099999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1893,7 +2531,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1925,7 +2563,7 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1966,7 +2604,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -4196,7 +4834,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>115</v>
       </c>
@@ -4228,7 +4866,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>115</v>
       </c>
@@ -4260,7 +4898,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>115</v>
       </c>
@@ -4292,7 +4930,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>115</v>
       </c>
@@ -4324,7 +4962,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>115</v>
       </c>
@@ -4356,7 +4994,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>230</v>
       </c>
@@ -4397,7 +5035,7 @@
         <v>0.64300000000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>115</v>
       </c>
@@ -4429,7 +5067,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>115</v>
       </c>
@@ -4461,7 +5099,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>115</v>
       </c>
@@ -4493,7 +5131,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>115</v>
       </c>
@@ -4528,7 +5166,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>115</v>
       </c>
@@ -4561,35 +5199,1479 @@
       </c>
       <c r="M91" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>115</v>
+      </c>
+      <c r="C92" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
+        <v>183</v>
+      </c>
+      <c r="I92" t="s">
+        <v>239</v>
+      </c>
+      <c r="J92">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="K92">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="L92">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="M92" t="s">
+        <v>242</v>
+      </c>
+      <c r="P92" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>115</v>
+      </c>
+      <c r="C93" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" t="s">
+        <v>19</v>
+      </c>
+      <c r="F93" t="s">
+        <v>183</v>
+      </c>
+      <c r="I93" t="s">
+        <v>239</v>
+      </c>
+      <c r="J93">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="K93">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="L93">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="M93" t="s">
+        <v>245</v>
+      </c>
+      <c r="P93" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B94" t="s">
+        <v>115</v>
+      </c>
+      <c r="C94" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" t="s">
+        <v>19</v>
+      </c>
+      <c r="F94" t="s">
+        <v>183</v>
+      </c>
+      <c r="I94" t="s">
+        <v>239</v>
+      </c>
+      <c r="J94">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="K94">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="L94">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="M94" t="s">
+        <v>247</v>
+      </c>
+      <c r="P94" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>115</v>
+      </c>
+      <c r="C95" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" t="s">
+        <v>19</v>
+      </c>
+      <c r="F95" t="s">
+        <v>183</v>
+      </c>
+      <c r="I95" t="s">
+        <v>239</v>
+      </c>
+      <c r="J95">
+        <v>0.64</v>
+      </c>
+      <c r="K95">
+        <v>0.74</v>
+      </c>
+      <c r="L95">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="M95" t="s">
+        <v>248</v>
+      </c>
+      <c r="P95" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>115</v>
+      </c>
+      <c r="C96" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" t="s">
+        <v>19</v>
+      </c>
+      <c r="F96" t="s">
+        <v>183</v>
+      </c>
+      <c r="I96" t="s">
+        <v>239</v>
+      </c>
+      <c r="J96">
+        <v>0.64</v>
+      </c>
+      <c r="K96">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="L96">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="M96" t="s">
+        <v>250</v>
+      </c>
+      <c r="P96" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>115</v>
+      </c>
+      <c r="C97" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F97" t="s">
+        <v>183</v>
+      </c>
+      <c r="I97" t="s">
+        <v>239</v>
+      </c>
+      <c r="J97">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="K97">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="L97">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="M97" t="s">
+        <v>253</v>
+      </c>
+      <c r="P97" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B98" t="s">
+        <v>115</v>
+      </c>
+      <c r="C98" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" t="s">
+        <v>19</v>
+      </c>
+      <c r="F98" t="s">
+        <v>183</v>
+      </c>
+      <c r="I98" t="s">
+        <v>239</v>
+      </c>
+      <c r="J98">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="K98">
+        <v>0.76</v>
+      </c>
+      <c r="L98">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="M98" t="s">
+        <v>254</v>
+      </c>
+      <c r="P98" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
+        <v>183</v>
+      </c>
+      <c r="I99" t="s">
+        <v>239</v>
+      </c>
+      <c r="J99">
+        <v>0.65</v>
+      </c>
+      <c r="K99">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="L99">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="M99" t="s">
+        <v>257</v>
+      </c>
+      <c r="P99" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B100" t="s">
+        <v>115</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" t="s">
+        <v>19</v>
+      </c>
+      <c r="F100" t="s">
+        <v>183</v>
+      </c>
+      <c r="I100" t="s">
+        <v>239</v>
+      </c>
+      <c r="J100">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K100">
+        <v>0.75</v>
+      </c>
+      <c r="L100">
+        <v>0.68</v>
+      </c>
+      <c r="M100" t="s">
+        <v>259</v>
+      </c>
+      <c r="P100" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>265</v>
+      </c>
+      <c r="B101" t="s">
+        <v>115</v>
+      </c>
+      <c r="C101" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" t="s">
+        <v>19</v>
+      </c>
+      <c r="F101" t="s">
+        <v>183</v>
+      </c>
+      <c r="I101" t="s">
+        <v>239</v>
+      </c>
+      <c r="J101">
+        <v>0.64</v>
+      </c>
+      <c r="K101">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="L101">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="M101" t="s">
+        <v>260</v>
+      </c>
+      <c r="N101" t="s">
+        <v>264</v>
+      </c>
+      <c r="O101">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="P101" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B102" t="s">
+        <v>115</v>
+      </c>
+      <c r="C102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" t="s">
+        <v>183</v>
+      </c>
+      <c r="I102" t="s">
+        <v>239</v>
+      </c>
+      <c r="J102">
+        <v>0.63</v>
+      </c>
+      <c r="K102">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="L102">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="M102" t="s">
+        <v>262</v>
+      </c>
+      <c r="P102" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B103" t="s">
+        <v>115</v>
+      </c>
+      <c r="C103" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" t="s">
+        <v>183</v>
+      </c>
+      <c r="I103" t="s">
+        <v>239</v>
+      </c>
+      <c r="J103">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="K103">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L103">
+        <v>0.68</v>
+      </c>
+      <c r="M103" t="s">
+        <v>266</v>
+      </c>
+      <c r="P103" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B104" t="s">
+        <v>115</v>
+      </c>
+      <c r="C104" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" t="s">
+        <v>183</v>
+      </c>
+      <c r="I104" t="s">
+        <v>239</v>
+      </c>
+      <c r="J104">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="K104">
+        <v>0.745</v>
+      </c>
+      <c r="L104">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M104" t="s">
+        <v>268</v>
+      </c>
+      <c r="P104" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>115</v>
+      </c>
+      <c r="C105" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" t="s">
+        <v>19</v>
+      </c>
+      <c r="F105" t="s">
+        <v>183</v>
+      </c>
+      <c r="I105" t="s">
+        <v>239</v>
+      </c>
+      <c r="J105">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="K105">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L105">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="M105" t="s">
+        <v>270</v>
+      </c>
+      <c r="P105" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B106" t="s">
+        <v>115</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" t="s">
+        <v>183</v>
+      </c>
+      <c r="I106" t="s">
+        <v>239</v>
+      </c>
+      <c r="J106">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="K106">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L106">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="M106" t="s">
+        <v>262</v>
+      </c>
+      <c r="P106" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
+        <v>115</v>
+      </c>
+      <c r="C107" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" t="s">
+        <v>19</v>
+      </c>
+      <c r="F107" t="s">
+        <v>183</v>
+      </c>
+      <c r="I107" t="s">
+        <v>239</v>
+      </c>
+      <c r="J107">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="K107">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="L107">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="M107" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="P107" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B108" t="s">
+        <v>115</v>
+      </c>
+      <c r="C108" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108" t="s">
+        <v>183</v>
+      </c>
+      <c r="I108" t="s">
+        <v>239</v>
+      </c>
+      <c r="J108">
+        <v>0.623</v>
+      </c>
+      <c r="K108">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L108">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="M108" t="s">
+        <v>275</v>
+      </c>
+      <c r="P108" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>115</v>
+      </c>
+      <c r="C109" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" t="s">
+        <v>19</v>
+      </c>
+      <c r="F109" t="s">
+        <v>183</v>
+      </c>
+      <c r="I109" t="s">
+        <v>239</v>
+      </c>
+      <c r="J109">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="K109">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="L109">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="M109" t="s">
+        <v>278</v>
+      </c>
+      <c r="P109" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B110" t="s">
+        <v>115</v>
+      </c>
+      <c r="C110" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" t="s">
+        <v>19</v>
+      </c>
+      <c r="F110" t="s">
+        <v>183</v>
+      </c>
+      <c r="I110" t="s">
+        <v>239</v>
+      </c>
+      <c r="J110">
+        <v>0.621</v>
+      </c>
+      <c r="K110">
+        <v>0.753</v>
+      </c>
+      <c r="L110">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="M110" t="s">
+        <v>279</v>
+      </c>
+      <c r="P110" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>115</v>
+      </c>
+      <c r="C111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" t="s">
+        <v>183</v>
+      </c>
+      <c r="I111" t="s">
+        <v>239</v>
+      </c>
+      <c r="J111">
+        <v>0.62</v>
+      </c>
+      <c r="K111">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="L111">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="M111" t="s">
+        <v>281</v>
+      </c>
+      <c r="P111" s="5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B112" t="s">
+        <v>115</v>
+      </c>
+      <c r="C112" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" t="s">
+        <v>19</v>
+      </c>
+      <c r="F112" t="s">
+        <v>183</v>
+      </c>
+      <c r="I112" t="s">
+        <v>239</v>
+      </c>
+      <c r="J112">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="K112">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="L112">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="M112" t="s">
+        <v>284</v>
+      </c>
+      <c r="P112" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
+        <v>115</v>
+      </c>
+      <c r="C113" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" t="s">
+        <v>19</v>
+      </c>
+      <c r="F113" t="s">
+        <v>183</v>
+      </c>
+      <c r="I113" t="s">
+        <v>239</v>
+      </c>
+      <c r="J113">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="K113">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="L113">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M113" t="s">
+        <v>285</v>
+      </c>
+      <c r="P113" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="114" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
+        <v>115</v>
+      </c>
+      <c r="C114" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" t="s">
+        <v>19</v>
+      </c>
+      <c r="F114" t="s">
+        <v>183</v>
+      </c>
+      <c r="I114" t="s">
+        <v>239</v>
+      </c>
+      <c r="J114">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="K114">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="L114">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="M114" t="s">
+        <v>286</v>
+      </c>
+      <c r="P114" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="115" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B115" t="s">
+        <v>115</v>
+      </c>
+      <c r="C115" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" t="s">
+        <v>19</v>
+      </c>
+      <c r="F115" t="s">
+        <v>183</v>
+      </c>
+      <c r="I115" t="s">
+        <v>239</v>
+      </c>
+      <c r="J115">
+        <v>0.62</v>
+      </c>
+      <c r="K115">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L115">
+        <v>0.71</v>
+      </c>
+      <c r="M115" t="s">
+        <v>289</v>
+      </c>
+      <c r="P115" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="116" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>115</v>
+      </c>
+      <c r="C116" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" t="s">
+        <v>19</v>
+      </c>
+      <c r="F116" t="s">
+        <v>183</v>
+      </c>
+      <c r="I116" t="s">
+        <v>239</v>
+      </c>
+      <c r="J116">
+        <v>0.626</v>
+      </c>
+      <c r="K116">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="L116">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="M116" t="s">
+        <v>290</v>
+      </c>
+      <c r="P116" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="117" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>115</v>
+      </c>
+      <c r="C117" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" t="s">
+        <v>19</v>
+      </c>
+      <c r="F117" t="s">
+        <v>183</v>
+      </c>
+      <c r="I117" t="s">
+        <v>239</v>
+      </c>
+      <c r="J117">
+        <v>0.628</v>
+      </c>
+      <c r="K117">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="L117">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="M117" t="s">
+        <v>293</v>
+      </c>
+      <c r="P117" s="5" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="118" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
+        <v>115</v>
+      </c>
+      <c r="C118" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" t="s">
+        <v>19</v>
+      </c>
+      <c r="F118" t="s">
+        <v>183</v>
+      </c>
+      <c r="I118" t="s">
+        <v>239</v>
+      </c>
+      <c r="J118">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="K118">
+        <v>0.77</v>
+      </c>
+      <c r="L118">
+        <v>0.69</v>
+      </c>
+      <c r="M118" t="s">
+        <v>295</v>
+      </c>
+      <c r="P118" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="119" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
+        <v>115</v>
+      </c>
+      <c r="C119" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" t="s">
+        <v>19</v>
+      </c>
+      <c r="F119" t="s">
+        <v>183</v>
+      </c>
+      <c r="I119" t="s">
+        <v>239</v>
+      </c>
+      <c r="J119">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K119">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="L119">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="M119" t="s">
+        <v>296</v>
+      </c>
+      <c r="P119" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="120" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B120" t="s">
+        <v>115</v>
+      </c>
+      <c r="C120" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" t="s">
+        <v>19</v>
+      </c>
+      <c r="F120" t="s">
+        <v>183</v>
+      </c>
+      <c r="I120" t="s">
+        <v>239</v>
+      </c>
+      <c r="J120">
+        <v>0.63</v>
+      </c>
+      <c r="K120">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L120">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="M120" t="s">
+        <v>299</v>
+      </c>
+      <c r="P120" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="121" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B121" t="s">
+        <v>115</v>
+      </c>
+      <c r="C121" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" t="s">
+        <v>19</v>
+      </c>
+      <c r="F121" t="s">
+        <v>183</v>
+      </c>
+      <c r="I121" t="s">
+        <v>239</v>
+      </c>
+      <c r="J121">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="K121">
+        <v>0.754</v>
+      </c>
+      <c r="L121">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="M121" t="s">
+        <v>301</v>
+      </c>
+      <c r="P121" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="122" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B122" t="s">
+        <v>115</v>
+      </c>
+      <c r="C122" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" t="s">
+        <v>19</v>
+      </c>
+      <c r="F122" t="s">
+        <v>183</v>
+      </c>
+      <c r="I122" t="s">
+        <v>239</v>
+      </c>
+      <c r="J122">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K122">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="L122">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="M122" t="s">
+        <v>302</v>
+      </c>
+      <c r="P122" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="123" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B123" t="s">
+        <v>115</v>
+      </c>
+      <c r="C123" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" t="s">
+        <v>19</v>
+      </c>
+      <c r="F123" t="s">
+        <v>183</v>
+      </c>
+      <c r="I123" t="s">
+        <v>239</v>
+      </c>
+      <c r="J123">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="K123">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="L123">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="M123" t="s">
+        <v>305</v>
+      </c>
+      <c r="P123" s="5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="124" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B124" t="s">
+        <v>115</v>
+      </c>
+      <c r="C124" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" t="s">
+        <v>19</v>
+      </c>
+      <c r="F124" t="s">
+        <v>183</v>
+      </c>
+      <c r="I124" t="s">
+        <v>239</v>
+      </c>
+      <c r="J124">
+        <v>0.627</v>
+      </c>
+      <c r="K124">
+        <v>0.746</v>
+      </c>
+      <c r="L124">
+        <v>0.7</v>
+      </c>
+      <c r="M124" t="s">
+        <v>307</v>
+      </c>
+      <c r="P124" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="125" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B125" t="s">
+        <v>115</v>
+      </c>
+      <c r="C125" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" t="s">
+        <v>19</v>
+      </c>
+      <c r="F125" t="s">
+        <v>183</v>
+      </c>
+      <c r="I125" t="s">
+        <v>239</v>
+      </c>
+      <c r="J125">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="K125">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L125">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="M125" t="s">
+        <v>309</v>
+      </c>
+      <c r="P125" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="126" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B126" t="s">
+        <v>115</v>
+      </c>
+      <c r="C126" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" t="s">
+        <v>19</v>
+      </c>
+      <c r="F126" t="s">
+        <v>183</v>
+      </c>
+      <c r="I126" t="s">
+        <v>239</v>
+      </c>
+      <c r="J126">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="K126">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L126">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="M126" t="s">
+        <v>310</v>
+      </c>
+      <c r="P126" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="127" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
+        <v>115</v>
+      </c>
+      <c r="C127" t="s">
+        <v>11</v>
+      </c>
+      <c r="D127" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" t="s">
+        <v>19</v>
+      </c>
+      <c r="F127" t="s">
+        <v>183</v>
+      </c>
+      <c r="I127" t="s">
+        <v>239</v>
+      </c>
+      <c r="J127">
+        <v>0.62</v>
+      </c>
+      <c r="K127">
+        <v>0.753</v>
+      </c>
+      <c r="L127">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="M127" t="s">
+        <v>312</v>
+      </c>
+      <c r="P127" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="128" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
+        <v>115</v>
+      </c>
+      <c r="C128" t="s">
+        <v>11</v>
+      </c>
+      <c r="D128" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" t="s">
+        <v>19</v>
+      </c>
+      <c r="F128" t="s">
+        <v>183</v>
+      </c>
+      <c r="I128" t="s">
+        <v>239</v>
+      </c>
+      <c r="J128">
+        <v>0.628</v>
+      </c>
+      <c r="K128">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="L128">
+        <v>0.67</v>
+      </c>
+      <c r="M128" t="s">
+        <v>315</v>
+      </c>
+      <c r="P128" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="129" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B129" t="s">
+        <v>115</v>
+      </c>
+      <c r="C129" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" t="s">
+        <v>19</v>
+      </c>
+      <c r="F129" t="s">
+        <v>183</v>
+      </c>
+      <c r="I129" t="s">
+        <v>239</v>
+      </c>
+      <c r="J129">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="K129">
+        <v>0.745</v>
+      </c>
+      <c r="L129">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="M129" t="s">
+        <v>316</v>
+      </c>
+      <c r="P129" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="130" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B130" t="s">
+        <v>115</v>
+      </c>
+      <c r="C130" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" t="s">
+        <v>19</v>
+      </c>
+      <c r="F130" t="s">
+        <v>183</v>
+      </c>
+      <c r="I130" t="s">
+        <v>239</v>
+      </c>
+      <c r="J130">
+        <v>0.63</v>
+      </c>
+      <c r="K130">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L130">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="M130" t="s">
+        <v>319</v>
+      </c>
+      <c r="P130" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="131" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B131" t="s">
+        <v>115</v>
+      </c>
+      <c r="C131" t="s">
+        <v>11</v>
+      </c>
+      <c r="D131" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" t="s">
+        <v>19</v>
+      </c>
+      <c r="F131" t="s">
+        <v>183</v>
+      </c>
+      <c r="I131" t="s">
+        <v>239</v>
+      </c>
+      <c r="J131">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="K131">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="L131">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="M131" t="s">
+        <v>320</v>
+      </c>
+      <c r="P131" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="132" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B132" t="s">
+        <v>115</v>
+      </c>
+      <c r="C132" t="s">
+        <v>11</v>
+      </c>
+      <c r="D132" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" t="s">
+        <v>19</v>
+      </c>
+      <c r="F132" t="s">
+        <v>183</v>
+      </c>
+      <c r="I132" t="s">
+        <v>239</v>
+      </c>
+      <c r="J132">
+        <v>0.63</v>
+      </c>
+      <c r="K132">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="L132">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="M132" t="s">
+        <v>322</v>
+      </c>
+      <c r="P132" s="5" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="25" priority="6" rank="1"/>
-    <cfRule type="top10" dxfId="24" priority="11" rank="2"/>
+    <cfRule type="top10" dxfId="15" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="11" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="23" priority="5" rank="1"/>
-    <cfRule type="top10" dxfId="22" priority="10" rank="2"/>
+    <cfRule type="top10" dxfId="13" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="10" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="top10" dxfId="21" priority="4" rank="1"/>
+  <conditionalFormatting sqref="K1:K122 K124:K1048576">
+    <cfRule type="top10" dxfId="11" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="20" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="3" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K91">
-    <cfRule type="top10" dxfId="19" priority="9" rank="2"/>
+  <conditionalFormatting sqref="K2:K122 K124:K128">
+    <cfRule type="top10" dxfId="9" priority="9" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J91">
-    <cfRule type="top10" dxfId="18" priority="8" rank="2"/>
+  <conditionalFormatting sqref="J2:J134">
+    <cfRule type="top10" dxfId="8" priority="8" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="17" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="16" priority="2" rank="2"/>
+    <cfRule type="top10" dxfId="6" priority="2" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
tuning results for agg MoCo features
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489970A6-186C-2647-845E-45D552D67D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8379D0E3-3CB2-1D46-A61E-E147EE554868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
+    <workbookView xWindow="1040" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="391">
   <si>
     <t>Model</t>
   </si>
@@ -1588,6 +1588,99 @@
   </si>
   <si>
     <t>0.738 (0.054)</t>
+  </si>
+  <si>
+    <t>0.753 (0.039)</t>
+  </si>
+  <si>
+    <t>{'random_strength': 4}</t>
+  </si>
+  <si>
+    <t>2023-03-22-1856_Catboost_manualdupes_Standard_featselect01_randomstrength4.csv</t>
+  </si>
+  <si>
+    <t>{'C': 3}</t>
+  </si>
+  <si>
+    <t>0.758 (0.047)</t>
+  </si>
+  <si>
+    <t>2023-03-22-2027_SVM_manualdupes_standard_featselect01.csv</t>
+  </si>
+  <si>
+    <t>0.771 (0.071)</t>
+  </si>
+  <si>
+    <t>2023-03-22-2059_SVM_manualdupes_standard_featselect01_tuned.csv</t>
+  </si>
+  <si>
+    <t>manual dupes, standard scaling, feature selection &gt; 0.1, tuned</t>
+  </si>
+  <si>
+    <t>2023-03-22-2133_LogReg_manualdupes_standard_featselect01.csv</t>
+  </si>
+  <si>
+    <t>0.699 (0.066)</t>
+  </si>
+  <si>
+    <t>2023-03-22-2201_LightGBM_manualdupes_standard_featselect01.csv</t>
+  </si>
+  <si>
+    <t>0.707 (0.056)</t>
+  </si>
+  <si>
+    <t>2023-03-22-2304_XGB_manualdupes_standard_featselect01.csv</t>
+  </si>
+  <si>
+    <t>March 22, 2023, 10:04 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-23-0406_RF_manualdupes_standard_featselect01.csv</t>
+  </si>
+  <si>
+    <t>2023-03-23-0418_ExtraTrees_manualdupes_standard_featselect01.csv</t>
+  </si>
+  <si>
+    <t>0.738 (0.037)</t>
+  </si>
+  <si>
+    <t>0.716 (0.012)</t>
+  </si>
+  <si>
+    <t>{'alpha': 2, 'lambda': 3,  'learning_rate': 0.3,  'max_depth': 4}</t>
+  </si>
+  <si>
+    <t>0.725 (0.065)</t>
+  </si>
+  <si>
+    <t>2023-03-23-0615_XGB_manualdupes_standard_featselect01_tuned.csv</t>
+  </si>
+  <si>
+    <t>March 23, 2023, 12:11 p.m.</t>
+  </si>
+  <si>
+    <t>2023-03-23-1033_LightGBM_manualdupes_standard_featselect01_tuned.csv</t>
+  </si>
+  <si>
+    <t>0.756 (0.057)</t>
+  </si>
+  <si>
+    <t>{'extra_trees': True, 'lambda_l1': 0.5, 'lambda_l2': 0, 'learning_rate': 0.2, 'max_depth': 6, 'path_smooth': 0}</t>
+  </si>
+  <si>
+    <t>{'ccp_alpha': 0, 'max_depth': 6, 'max_features': 1, 'n_estimators': 300}</t>
+  </si>
+  <si>
+    <t>0.741 (0.019)</t>
+  </si>
+  <si>
+    <t>2023-03-23-1342_ExtraTrees_manualdupes_standard_featselect01_tuned.csv</t>
+  </si>
+  <si>
+    <t>0.735 (0.026)</t>
+  </si>
+  <si>
+    <t>2023-03-23-1438_RandomForest_manualdupes_standard_featselect01_tuned.csv</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1712,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1629,6 +1722,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1656,7 +1755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1667,6 +1766,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1684,21 +1784,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1786,8 +1886,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P149" totalsRowShown="0">
-  <autoFilter ref="A1:P149" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P161" totalsRowShown="0">
+  <autoFilter ref="A1:P161" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -2107,10 +2207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:P149"/>
+  <dimension ref="A1:P161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P152" sqref="P152"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7104,7 +7204,7 @@
       <c r="A144" t="s">
         <v>344</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C144" t="s">
@@ -7122,16 +7222,16 @@
       <c r="I144" t="s">
         <v>342</v>
       </c>
-      <c r="J144" s="5">
+      <c r="J144">
         <v>0.67700000000000005</v>
       </c>
-      <c r="K144" s="5">
+      <c r="K144">
         <v>0.78600000000000003</v>
       </c>
-      <c r="L144" s="5">
+      <c r="L144">
         <v>0.73299999999999998</v>
       </c>
-      <c r="M144" s="5" t="s">
+      <c r="M144" t="s">
         <v>343</v>
       </c>
       <c r="N144" t="s">
@@ -7331,6 +7431,501 @@
         <v>359</v>
       </c>
       <c r="P149" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>362</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C150" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" t="s">
+        <v>19</v>
+      </c>
+      <c r="F150" t="s">
+        <v>183</v>
+      </c>
+      <c r="H150" t="s">
+        <v>361</v>
+      </c>
+      <c r="I150" t="s">
+        <v>368</v>
+      </c>
+      <c r="J150">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="K150">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="L150">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="M150" t="s">
+        <v>360</v>
+      </c>
+      <c r="O150">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="P150" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>365</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C151" t="s">
+        <v>11</v>
+      </c>
+      <c r="D151" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" t="s">
+        <v>19</v>
+      </c>
+      <c r="F151" t="s">
+        <v>183</v>
+      </c>
+      <c r="I151" t="s">
+        <v>328</v>
+      </c>
+      <c r="J151">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="K151">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="L151">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="M151" t="s">
+        <v>364</v>
+      </c>
+      <c r="N151" t="s">
+        <v>374</v>
+      </c>
+      <c r="O151">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="P151" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>367</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C152" t="s">
+        <v>11</v>
+      </c>
+      <c r="D152" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" t="s">
+        <v>19</v>
+      </c>
+      <c r="F152" t="s">
+        <v>183</v>
+      </c>
+      <c r="H152" t="s">
+        <v>363</v>
+      </c>
+      <c r="I152" t="s">
+        <v>368</v>
+      </c>
+      <c r="J152">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="K152">
+        <v>0.871</v>
+      </c>
+      <c r="L152">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="M152" t="s">
+        <v>366</v>
+      </c>
+      <c r="N152" t="s">
+        <v>382</v>
+      </c>
+      <c r="O152">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="P152" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>369</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C153" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" t="s">
+        <v>8</v>
+      </c>
+      <c r="E153" t="s">
+        <v>19</v>
+      </c>
+      <c r="F153" t="s">
+        <v>183</v>
+      </c>
+      <c r="I153" t="s">
+        <v>328</v>
+      </c>
+      <c r="J153">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="K153">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="L153">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="M153" t="s">
+        <v>359</v>
+      </c>
+      <c r="P153" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>373</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C154" t="s">
+        <v>11</v>
+      </c>
+      <c r="D154" t="s">
+        <v>8</v>
+      </c>
+      <c r="E154" t="s">
+        <v>19</v>
+      </c>
+      <c r="F154" t="s">
+        <v>183</v>
+      </c>
+      <c r="I154" t="s">
+        <v>328</v>
+      </c>
+      <c r="J154">
+        <v>0.629</v>
+      </c>
+      <c r="K154">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="L154">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="M154" t="s">
+        <v>372</v>
+      </c>
+      <c r="P154" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>376</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C155" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" t="s">
+        <v>19</v>
+      </c>
+      <c r="F155" t="s">
+        <v>183</v>
+      </c>
+      <c r="H155" t="s">
+        <v>338</v>
+      </c>
+      <c r="I155" t="s">
+        <v>328</v>
+      </c>
+      <c r="J155">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="K155">
+        <v>0.755</v>
+      </c>
+      <c r="L155">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="M155" t="s">
+        <v>377</v>
+      </c>
+      <c r="P155" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>375</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C156" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" t="s">
+        <v>19</v>
+      </c>
+      <c r="F156" t="s">
+        <v>183</v>
+      </c>
+      <c r="H156" t="s">
+        <v>338</v>
+      </c>
+      <c r="I156" t="s">
+        <v>328</v>
+      </c>
+      <c r="J156">
+        <v>0.7</v>
+      </c>
+      <c r="K156">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="L156">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="M156" t="s">
+        <v>378</v>
+      </c>
+      <c r="P156" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>371</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C157" t="s">
+        <v>11</v>
+      </c>
+      <c r="D157" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" t="s">
+        <v>19</v>
+      </c>
+      <c r="F157" t="s">
+        <v>183</v>
+      </c>
+      <c r="I157" t="s">
+        <v>328</v>
+      </c>
+      <c r="J157">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="K157">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="L157">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="M157" t="s">
+        <v>370</v>
+      </c>
+      <c r="P157" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>381</v>
+      </c>
+      <c r="B158" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C158" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" t="s">
+        <v>19</v>
+      </c>
+      <c r="F158" t="s">
+        <v>183</v>
+      </c>
+      <c r="H158" t="s">
+        <v>379</v>
+      </c>
+      <c r="I158" t="s">
+        <v>368</v>
+      </c>
+      <c r="J158">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="K158">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="L158">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="M158" t="s">
+        <v>380</v>
+      </c>
+      <c r="P158" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>388</v>
+      </c>
+      <c r="B159" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C159" t="s">
+        <v>11</v>
+      </c>
+      <c r="D159" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" t="s">
+        <v>19</v>
+      </c>
+      <c r="F159" t="s">
+        <v>183</v>
+      </c>
+      <c r="H159" t="s">
+        <v>386</v>
+      </c>
+      <c r="I159" t="s">
+        <v>368</v>
+      </c>
+      <c r="J159">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="K159">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="L159">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="M159" t="s">
+        <v>387</v>
+      </c>
+      <c r="P159" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>390</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C160" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" t="s">
+        <v>19</v>
+      </c>
+      <c r="F160" t="s">
+        <v>183</v>
+      </c>
+      <c r="H160" t="s">
+        <v>386</v>
+      </c>
+      <c r="I160" t="s">
+        <v>368</v>
+      </c>
+      <c r="J160">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="K160">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="L160">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="M160" t="s">
+        <v>389</v>
+      </c>
+      <c r="P160" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>383</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C161" t="s">
+        <v>11</v>
+      </c>
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" t="s">
+        <v>19</v>
+      </c>
+      <c r="F161" t="s">
+        <v>183</v>
+      </c>
+      <c r="H161" t="s">
+        <v>385</v>
+      </c>
+      <c r="I161" t="s">
+        <v>368</v>
+      </c>
+      <c r="J161">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="K161">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="L161">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="M161" t="s">
+        <v>384</v>
+      </c>
+      <c r="P161" s="5" t="s">
         <v>308</v>
       </c>
     </row>
@@ -7353,14 +7948,14 @@
   <conditionalFormatting sqref="K2:K122 K124:K128">
     <cfRule type="top10" dxfId="3" priority="9" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J149">
-    <cfRule type="top10" dxfId="2" priority="8" rank="2"/>
+  <conditionalFormatting sqref="M67">
+    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="2" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="0" priority="2" rank="2"/>
+  <conditionalFormatting sqref="J2:J161">
+    <cfRule type="top10" dxfId="0" priority="53" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
implemented stacking for training and submission
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8379D0E3-3CB2-1D46-A61E-E147EE554868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0A1BF8-13BB-954C-9F54-4FEFD57BDDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="397">
   <si>
     <t>Model</t>
   </si>
@@ -1681,6 +1681,24 @@
   </si>
   <si>
     <t>2023-03-23-1438_RandomForest_manualdupes_standard_featselect01_tuned.csv</t>
+  </si>
+  <si>
+    <t>March 23, 2023, 2:48 p.m.</t>
+  </si>
+  <si>
+    <t>March 23, 2023, 2:49 p.m.</t>
+  </si>
+  <si>
+    <t>Stacking</t>
+  </si>
+  <si>
+    <t>RF: {"max_features": 1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.759 (0.033)</t>
+  </si>
+  <si>
+    <t>"['RF', 'SVM', 'Catboost']", manual dupes, standard scaling, feature selection &gt; 0.1</t>
   </si>
 </sst>
 </file>
@@ -1886,8 +1904,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P161" totalsRowShown="0">
-  <autoFilter ref="A1:P161" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P162" totalsRowShown="0">
+  <autoFilter ref="A1:P162" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -2207,10 +2225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:P161"/>
+  <dimension ref="A1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+    <sheetView tabSelected="1" topLeftCell="B130" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O163" sqref="O163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7603,6 +7621,9 @@
       <c r="M153" t="s">
         <v>359</v>
       </c>
+      <c r="O153">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="P153" s="5" t="s">
         <v>308</v>
       </c>
@@ -7641,6 +7662,9 @@
       <c r="M154" t="s">
         <v>372</v>
       </c>
+      <c r="O154">
+        <v>0.60299999999999998</v>
+      </c>
       <c r="P154" s="5" t="s">
         <v>308</v>
       </c>
@@ -7682,6 +7706,9 @@
       <c r="M155" t="s">
         <v>377</v>
       </c>
+      <c r="O155">
+        <v>0.627</v>
+      </c>
       <c r="P155" s="5" t="s">
         <v>308</v>
       </c>
@@ -7723,6 +7750,12 @@
       <c r="M156" t="s">
         <v>378</v>
       </c>
+      <c r="N156" t="s">
+        <v>391</v>
+      </c>
+      <c r="O156">
+        <v>0.71</v>
+      </c>
       <c r="P156" s="5" t="s">
         <v>308</v>
       </c>
@@ -7761,6 +7794,9 @@
       <c r="M157" t="s">
         <v>370</v>
       </c>
+      <c r="O157">
+        <v>0.63600000000000001</v>
+      </c>
       <c r="P157" s="5" t="s">
         <v>308</v>
       </c>
@@ -7802,6 +7838,9 @@
       <c r="M158" t="s">
         <v>380</v>
       </c>
+      <c r="O158">
+        <v>0.6</v>
+      </c>
       <c r="P158" s="5" t="s">
         <v>308</v>
       </c>
@@ -7843,6 +7882,9 @@
       <c r="M159" t="s">
         <v>387</v>
       </c>
+      <c r="O159">
+        <v>0.63100000000000001</v>
+      </c>
       <c r="P159" s="5" t="s">
         <v>308</v>
       </c>
@@ -7884,6 +7926,12 @@
       <c r="M160" t="s">
         <v>389</v>
       </c>
+      <c r="N160" t="s">
+        <v>392</v>
+      </c>
+      <c r="O160">
+        <v>0.65100000000000002</v>
+      </c>
       <c r="P160" s="5" t="s">
         <v>308</v>
       </c>
@@ -7925,8 +7973,49 @@
       <c r="M161" t="s">
         <v>384</v>
       </c>
+      <c r="O161">
+        <v>0.59299999999999997</v>
+      </c>
       <c r="P161" s="5" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B162" t="s">
+        <v>393</v>
+      </c>
+      <c r="C162" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" t="s">
+        <v>8</v>
+      </c>
+      <c r="E162" t="s">
+        <v>19</v>
+      </c>
+      <c r="F162" t="s">
+        <v>183</v>
+      </c>
+      <c r="H162" t="s">
+        <v>394</v>
+      </c>
+      <c r="I162" t="s">
+        <v>396</v>
+      </c>
+      <c r="J162">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="K162">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="L162">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="M162" t="s">
+        <v>395</v>
+      </c>
+      <c r="O162">
+        <v>0.63900000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -7954,7 +8043,7 @@
   <conditionalFormatting sqref="M67">
     <cfRule type="top10" dxfId="1" priority="2" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J161">
+  <conditionalFormatting sqref="J2:J162">
     <cfRule type="top10" dxfId="0" priority="53" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finalised tracking of models
</commit_message>
<xml_diff>
--- a/modeling/Overview_Modeling.xlsx
+++ b/modeling/Overview_Modeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0A1BF8-13BB-954C-9F54-4FEFD57BDDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83155BC5-E8E8-8044-AE53-6FB5FF3A24D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="760" windowWidth="28240" windowHeight="17140" xr2:uid="{325DED77-4E3F-3240-BC23-3B02E9044B3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="412">
   <si>
     <t>Model</t>
   </si>
@@ -1699,6 +1699,51 @@
   </si>
   <si>
     <t>"['RF', 'SVM', 'Catboost']", manual dupes, standard scaling, feature selection &gt; 0.1</t>
+  </si>
+  <si>
+    <t>0.678 (0.033)</t>
+  </si>
+  <si>
+    <t>manual dupes, standard scaling</t>
+  </si>
+  <si>
+    <t>standard scaling</t>
+  </si>
+  <si>
+    <t>0.644 (0.054)</t>
+  </si>
+  <si>
+    <t>0.609 (0.027)</t>
+  </si>
+  <si>
+    <t>2023-03-28-1949_RF_weakly_final_model.csv</t>
+  </si>
+  <si>
+    <t>0.734 (0.048)</t>
+  </si>
+  <si>
+    <t>2023-03-28-1934_Catboost_weakly_final_model.csv</t>
+  </si>
+  <si>
+    <t>0.741 (0.055)</t>
+  </si>
+  <si>
+    <t>0.700 (0.027)</t>
+  </si>
+  <si>
+    <t>2023-03-29-2018_LGBM_weakly_final_model.csv</t>
+  </si>
+  <si>
+    <t>2023-03-28-2349_ET_weakly_final_model.csv</t>
+  </si>
+  <si>
+    <t>2023-03-28-2250_XGB_weakly_final_model.csv</t>
+  </si>
+  <si>
+    <t>2023-03-28-2147_LogReg_weakly_final_model.csv</t>
+  </si>
+  <si>
+    <t>0.712 (0.049)</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1834,37 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1904,8 +1979,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P162" totalsRowShown="0">
-  <autoFilter ref="A1:P162" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}" name="Tabelle1" displayName="Tabelle1" ref="A1:P170" totalsRowShown="0">
+  <autoFilter ref="A1:P170" xr:uid="{BD928D43-FFBC-4B44-A1D4-6A08A8FDC4D9}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{4F09B17A-AEA7-A249-B731-CBDD1A1B4321}" name="File"/>
     <tableColumn id="2" xr3:uid="{097273E9-4D4D-2D48-B70B-ADFDE72AE62C}" name="Model"/>
@@ -2225,10 +2300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC34F2-1233-B044-BEAC-F5D19B0E9201}">
-  <dimension ref="A1:P162"/>
+  <dimension ref="A1:P170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B130" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O163" sqref="O163"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L171" sqref="L171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8018,33 +8093,319 @@
         <v>0.63900000000000001</v>
       </c>
     </row>
+    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>404</v>
+      </c>
+      <c r="B163" t="s">
+        <v>115</v>
+      </c>
+      <c r="C163" t="s">
+        <v>11</v>
+      </c>
+      <c r="D163" t="s">
+        <v>8</v>
+      </c>
+      <c r="E163" t="s">
+        <v>19</v>
+      </c>
+      <c r="F163" t="s">
+        <v>40</v>
+      </c>
+      <c r="I163" t="s">
+        <v>328</v>
+      </c>
+      <c r="J163">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="K163">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="L163">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="M163" t="s">
+        <v>397</v>
+      </c>
+      <c r="O163">
+        <v>0.60299999999999998</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B164" t="s">
+        <v>115</v>
+      </c>
+      <c r="C164" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164" t="s">
+        <v>8</v>
+      </c>
+      <c r="E164" t="s">
+        <v>19</v>
+      </c>
+      <c r="F164" t="s">
+        <v>40</v>
+      </c>
+      <c r="I164" t="s">
+        <v>398</v>
+      </c>
+      <c r="J164">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="K164">
+        <v>0.72</v>
+      </c>
+      <c r="L164">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="M164" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
+        <v>115</v>
+      </c>
+      <c r="C165" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" t="s">
+        <v>8</v>
+      </c>
+      <c r="E165" t="s">
+        <v>19</v>
+      </c>
+      <c r="F165" t="s">
+        <v>40</v>
+      </c>
+      <c r="I165" t="s">
+        <v>399</v>
+      </c>
+      <c r="J165">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="K165">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="L165">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="M165" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>402</v>
+      </c>
+      <c r="B166" t="s">
+        <v>38</v>
+      </c>
+      <c r="C166" t="s">
+        <v>11</v>
+      </c>
+      <c r="D166" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" t="s">
+        <v>19</v>
+      </c>
+      <c r="F166" t="s">
+        <v>40</v>
+      </c>
+      <c r="I166" t="s">
+        <v>328</v>
+      </c>
+      <c r="J166">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="K166">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="L166">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="M166" t="s">
+        <v>403</v>
+      </c>
+      <c r="O166">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>410</v>
+      </c>
+      <c r="B167" t="s">
+        <v>35</v>
+      </c>
+      <c r="C167" t="s">
+        <v>11</v>
+      </c>
+      <c r="D167" t="s">
+        <v>8</v>
+      </c>
+      <c r="E167" t="s">
+        <v>19</v>
+      </c>
+      <c r="F167" t="s">
+        <v>40</v>
+      </c>
+      <c r="I167" t="s">
+        <v>328</v>
+      </c>
+      <c r="J167">
+        <v>0.627</v>
+      </c>
+      <c r="K167">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="L167">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="M167" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>409</v>
+      </c>
+      <c r="B168" t="s">
+        <v>37</v>
+      </c>
+      <c r="C168" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" t="s">
+        <v>8</v>
+      </c>
+      <c r="E168" t="s">
+        <v>19</v>
+      </c>
+      <c r="F168" t="s">
+        <v>40</v>
+      </c>
+      <c r="I168" t="s">
+        <v>328</v>
+      </c>
+      <c r="J168">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="K168">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="L168">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="M168" t="s">
+        <v>406</v>
+      </c>
+      <c r="O168">
+        <v>0.62980000000000003</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>408</v>
+      </c>
+      <c r="B169" t="s">
+        <v>118</v>
+      </c>
+      <c r="C169" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169" t="s">
+        <v>8</v>
+      </c>
+      <c r="E169" t="s">
+        <v>19</v>
+      </c>
+      <c r="F169" t="s">
+        <v>40</v>
+      </c>
+      <c r="I169" t="s">
+        <v>328</v>
+      </c>
+      <c r="J169">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="K169">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="L169">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="M169" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>407</v>
+      </c>
+      <c r="B170" t="s">
+        <v>117</v>
+      </c>
+      <c r="C170" t="s">
+        <v>11</v>
+      </c>
+      <c r="D170" t="s">
+        <v>8</v>
+      </c>
+      <c r="E170" t="s">
+        <v>19</v>
+      </c>
+      <c r="F170" t="s">
+        <v>40</v>
+      </c>
+      <c r="I170" t="s">
+        <v>328</v>
+      </c>
+      <c r="J170">
+        <v>0.66</v>
+      </c>
+      <c r="K170">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="L170">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="M170" t="s">
+        <v>411</v>
+      </c>
+      <c r="O170">
+        <v>0.58169999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="top10" dxfId="9" priority="6" rank="1"/>
-    <cfRule type="top10" dxfId="8" priority="11" rank="2"/>
+    <cfRule type="top10" dxfId="12" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="11" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="top10" dxfId="7" priority="5" rank="1"/>
-    <cfRule type="top10" dxfId="6" priority="10" rank="2"/>
+    <cfRule type="top10" dxfId="10" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="10" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K122 K146:K1048576 K124:K144">
-    <cfRule type="top10" dxfId="5" priority="4" rank="1"/>
+  <conditionalFormatting sqref="K1:K122 K146:K164 K166:K1048576 K124:K144">
+    <cfRule type="top10" dxfId="8" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="top10" dxfId="4" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K122 K124:K128">
-    <cfRule type="top10" dxfId="3" priority="9" rank="2"/>
+    <cfRule type="top10" dxfId="6" priority="9" rank="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="2" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M67">
-    <cfRule type="top10" dxfId="1" priority="2" rank="2"/>
+    <cfRule type="top10" dxfId="4" priority="2" rank="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J162">
-    <cfRule type="top10" dxfId="0" priority="53" rank="2"/>
+  <conditionalFormatting sqref="J2:J170">
+    <cfRule type="top10" dxfId="3" priority="53" rank="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>